<commit_message>
update progress bab 4
</commit_message>
<xml_diff>
--- a/HASIL PENGUJIAN 100 EPOCHS.xlsx
+++ b/HASIL PENGUJIAN 100 EPOCHS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SKRIPSI\Skripsi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D5210E-BE12-467C-B5B6-2F2B6B27A020}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A06F3461-43FB-4871-A55D-8E6D37DD32FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ADAM FULL" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="ADAM SMALL" sheetId="4" r:id="rId5"/>
     <sheet name="SGD SMALL" sheetId="5" r:id="rId6"/>
     <sheet name="RMSProp SMALL" sheetId="6" r:id="rId7"/>
+    <sheet name="Rekapan" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="34">
   <si>
     <t>80/20</t>
   </si>
@@ -113,12 +114,33 @@
   <si>
     <t>806.36 seconds.</t>
   </si>
+  <si>
+    <t>No.</t>
+  </si>
+  <si>
+    <t>Pembagian Data</t>
+  </si>
+  <si>
+    <t>Akurasi</t>
+  </si>
+  <si>
+    <t>f1-score</t>
+  </si>
+  <si>
+    <t>Precision</t>
+  </si>
+  <si>
+    <t>Recall</t>
+  </si>
+  <si>
+    <t>Durasi Training</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,6 +229,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -258,7 +286,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -346,11 +374,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -404,12 +443,26 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3177,15 +3230,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>186073</xdr:rowOff>
+      <xdr:colOff>380999</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>9180</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>207818</xdr:colOff>
+      <xdr:colOff>207817</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>23380</xdr:rowOff>
+      <xdr:rowOff>36987</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3215,8 +3268,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="987136" y="567073"/>
-          <a:ext cx="7706591" cy="2746762"/>
+          <a:off x="993320" y="580680"/>
+          <a:ext cx="7786997" cy="2749236"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3608,16 +3661,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="D4:AL83"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P26" sqref="P26"/>
+    <sheetView showGridLines="0" topLeftCell="A33" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:38">
+    <row r="4" spans="4:38" x14ac:dyDescent="0.25">
       <c r="X4" s="1" t="s">
         <v>3</v>
       </c>
@@ -3625,7 +3678,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="4:38">
+    <row r="6" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D6" s="2"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -3663,19 +3716,19 @@
       <c r="AK6" s="3"/>
       <c r="AL6" s="4"/>
     </row>
-    <row r="7" spans="4:38">
+    <row r="7" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D7" s="5"/>
       <c r="T7" s="6"/>
       <c r="V7" s="5"/>
       <c r="AL7" s="6"/>
     </row>
-    <row r="8" spans="4:38">
+    <row r="8" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D8" s="5"/>
       <c r="T8" s="6"/>
       <c r="V8" s="5"/>
       <c r="AL8" s="6"/>
     </row>
-    <row r="9" spans="4:38">
+    <row r="9" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D9" s="5"/>
       <c r="R9" s="31" t="s">
         <v>1</v>
@@ -3689,7 +3742,7 @@
       <c r="AK9" s="31"/>
       <c r="AL9" s="6"/>
     </row>
-    <row r="10" spans="4:38">
+    <row r="10" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D10" s="5"/>
       <c r="R10" s="32" t="s">
         <v>0</v>
@@ -3703,7 +3756,7 @@
       <c r="AK10" s="32"/>
       <c r="AL10" s="6"/>
     </row>
-    <row r="11" spans="4:38">
+    <row r="11" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D11" s="5"/>
       <c r="R11" s="32"/>
       <c r="S11" s="32"/>
@@ -3713,7 +3766,7 @@
       <c r="AK11" s="32"/>
       <c r="AL11" s="6"/>
     </row>
-    <row r="12" spans="4:38" ht="18.75">
+    <row r="12" spans="4:38" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D12" s="5"/>
       <c r="R12" s="33" t="s">
         <v>2</v>
@@ -3727,187 +3780,187 @@
       <c r="AK12" s="33"/>
       <c r="AL12" s="6"/>
     </row>
-    <row r="13" spans="4:38">
+    <row r="13" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D13" s="5"/>
       <c r="T13" s="6"/>
       <c r="V13" s="5"/>
       <c r="AL13" s="6"/>
     </row>
-    <row r="14" spans="4:38">
+    <row r="14" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D14" s="5"/>
       <c r="T14" s="6"/>
       <c r="V14" s="5"/>
       <c r="AL14" s="6"/>
     </row>
-    <row r="15" spans="4:38">
+    <row r="15" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D15" s="5"/>
       <c r="T15" s="6"/>
       <c r="V15" s="5"/>
       <c r="AL15" s="6"/>
     </row>
-    <row r="16" spans="4:38">
+    <row r="16" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D16" s="5"/>
       <c r="T16" s="6"/>
       <c r="V16" s="5"/>
       <c r="AL16" s="6"/>
     </row>
-    <row r="17" spans="4:38">
+    <row r="17" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D17" s="5"/>
       <c r="T17" s="6"/>
       <c r="V17" s="5"/>
       <c r="AL17" s="6"/>
     </row>
-    <row r="18" spans="4:38">
+    <row r="18" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D18" s="5"/>
       <c r="T18" s="6"/>
       <c r="V18" s="5"/>
       <c r="AL18" s="6"/>
     </row>
-    <row r="19" spans="4:38">
+    <row r="19" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D19" s="5"/>
       <c r="T19" s="6"/>
       <c r="V19" s="5"/>
       <c r="AL19" s="6"/>
     </row>
-    <row r="20" spans="4:38">
+    <row r="20" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D20" s="5"/>
       <c r="T20" s="6"/>
       <c r="V20" s="5"/>
       <c r="AL20" s="6"/>
     </row>
-    <row r="21" spans="4:38">
+    <row r="21" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D21" s="5"/>
       <c r="T21" s="6"/>
       <c r="V21" s="5"/>
       <c r="AL21" s="6"/>
     </row>
-    <row r="22" spans="4:38">
+    <row r="22" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D22" s="5"/>
       <c r="T22" s="6"/>
       <c r="V22" s="5"/>
       <c r="AL22" s="6"/>
     </row>
-    <row r="23" spans="4:38">
+    <row r="23" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D23" s="5"/>
       <c r="T23" s="6"/>
       <c r="V23" s="5"/>
       <c r="AL23" s="6"/>
     </row>
-    <row r="24" spans="4:38">
+    <row r="24" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D24" s="5"/>
       <c r="T24" s="6"/>
       <c r="V24" s="5"/>
       <c r="AL24" s="6"/>
     </row>
-    <row r="25" spans="4:38">
+    <row r="25" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D25" s="5"/>
       <c r="T25" s="6"/>
       <c r="V25" s="5"/>
       <c r="AL25" s="6"/>
     </row>
-    <row r="26" spans="4:38">
+    <row r="26" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D26" s="5"/>
       <c r="T26" s="6"/>
       <c r="V26" s="5"/>
       <c r="AL26" s="6"/>
     </row>
-    <row r="27" spans="4:38">
+    <row r="27" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D27" s="5"/>
       <c r="T27" s="6"/>
       <c r="V27" s="5"/>
       <c r="AL27" s="6"/>
     </row>
-    <row r="28" spans="4:38">
+    <row r="28" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D28" s="5"/>
       <c r="T28" s="6"/>
       <c r="V28" s="5"/>
       <c r="AL28" s="6"/>
     </row>
-    <row r="29" spans="4:38">
+    <row r="29" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D29" s="5"/>
       <c r="T29" s="6"/>
       <c r="V29" s="5"/>
       <c r="AL29" s="6"/>
     </row>
-    <row r="30" spans="4:38">
+    <row r="30" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D30" s="5"/>
       <c r="T30" s="6"/>
       <c r="V30" s="5"/>
       <c r="AL30" s="6"/>
     </row>
-    <row r="31" spans="4:38">
+    <row r="31" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D31" s="5"/>
       <c r="T31" s="6"/>
       <c r="V31" s="5"/>
       <c r="AL31" s="6"/>
     </row>
-    <row r="32" spans="4:38">
+    <row r="32" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D32" s="5"/>
       <c r="T32" s="6"/>
       <c r="V32" s="5"/>
       <c r="AL32" s="6"/>
     </row>
-    <row r="33" spans="4:38">
+    <row r="33" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D33" s="5"/>
       <c r="T33" s="6"/>
       <c r="V33" s="5"/>
       <c r="AL33" s="6"/>
     </row>
-    <row r="34" spans="4:38">
+    <row r="34" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D34" s="5"/>
       <c r="T34" s="6"/>
       <c r="V34" s="5"/>
       <c r="AL34" s="6"/>
     </row>
-    <row r="35" spans="4:38">
+    <row r="35" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D35" s="5"/>
       <c r="T35" s="6"/>
       <c r="V35" s="5"/>
       <c r="AL35" s="6"/>
     </row>
-    <row r="36" spans="4:38">
+    <row r="36" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D36" s="5"/>
       <c r="T36" s="6"/>
       <c r="V36" s="5"/>
       <c r="AL36" s="6"/>
     </row>
-    <row r="37" spans="4:38">
+    <row r="37" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D37" s="5"/>
       <c r="T37" s="6"/>
       <c r="V37" s="5"/>
       <c r="AL37" s="6"/>
     </row>
-    <row r="38" spans="4:38">
+    <row r="38" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D38" s="5"/>
       <c r="T38" s="6"/>
       <c r="V38" s="5"/>
       <c r="AL38" s="6"/>
     </row>
-    <row r="39" spans="4:38">
+    <row r="39" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D39" s="5"/>
       <c r="T39" s="6"/>
       <c r="V39" s="5"/>
       <c r="AL39" s="6"/>
     </row>
-    <row r="40" spans="4:38">
+    <row r="40" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D40" s="5"/>
       <c r="T40" s="6"/>
       <c r="V40" s="5"/>
       <c r="AL40" s="6"/>
     </row>
-    <row r="41" spans="4:38">
+    <row r="41" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D41" s="5"/>
       <c r="T41" s="6"/>
       <c r="V41" s="5"/>
       <c r="AL41" s="6"/>
     </row>
-    <row r="42" spans="4:38">
+    <row r="42" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D42" s="5"/>
       <c r="T42" s="6"/>
       <c r="V42" s="5"/>
       <c r="AL42" s="6"/>
     </row>
-    <row r="43" spans="4:38">
+    <row r="43" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D43" s="7"/>
       <c r="E43" s="8"/>
       <c r="F43" s="8"/>
@@ -3943,7 +3996,7 @@
       <c r="AK43" s="8"/>
       <c r="AL43" s="9"/>
     </row>
-    <row r="46" spans="4:38">
+    <row r="46" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D46" s="2"/>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
@@ -3962,18 +4015,18 @@
       <c r="S46" s="3"/>
       <c r="T46" s="4"/>
     </row>
-    <row r="47" spans="4:38">
+    <row r="47" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D47" s="5"/>
       <c r="E47" s="20" t="s">
         <v>8</v>
       </c>
       <c r="T47" s="6"/>
     </row>
-    <row r="48" spans="4:38">
+    <row r="48" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D48" s="5"/>
       <c r="T48" s="6"/>
     </row>
-    <row r="49" spans="4:20">
+    <row r="49" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D49" s="5"/>
       <c r="R49" s="31" t="s">
         <v>1</v>
@@ -3981,7 +4034,7 @@
       <c r="S49" s="31"/>
       <c r="T49" s="6"/>
     </row>
-    <row r="50" spans="4:20">
+    <row r="50" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D50" s="5"/>
       <c r="R50" s="32" t="s">
         <v>6</v>
@@ -3989,13 +4042,13 @@
       <c r="S50" s="32"/>
       <c r="T50" s="6"/>
     </row>
-    <row r="51" spans="4:20">
+    <row r="51" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D51" s="5"/>
       <c r="R51" s="32"/>
       <c r="S51" s="32"/>
       <c r="T51" s="6"/>
     </row>
-    <row r="52" spans="4:20" ht="18.75">
+    <row r="52" spans="4:20" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D52" s="5"/>
       <c r="R52" s="33" t="s">
         <v>2</v>
@@ -4003,67 +4056,67 @@
       <c r="S52" s="33"/>
       <c r="T52" s="6"/>
     </row>
-    <row r="53" spans="4:20">
+    <row r="53" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D53" s="5"/>
       <c r="T53" s="6"/>
     </row>
-    <row r="54" spans="4:20">
+    <row r="54" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D54" s="5"/>
       <c r="T54" s="6"/>
     </row>
-    <row r="55" spans="4:20">
+    <row r="55" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D55" s="5"/>
       <c r="T55" s="6"/>
     </row>
-    <row r="56" spans="4:20">
+    <row r="56" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D56" s="5"/>
       <c r="T56" s="6"/>
     </row>
-    <row r="57" spans="4:20">
+    <row r="57" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D57" s="5"/>
       <c r="T57" s="6"/>
     </row>
-    <row r="58" spans="4:20">
+    <row r="58" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D58" s="5"/>
       <c r="T58" s="6"/>
     </row>
-    <row r="59" spans="4:20">
+    <row r="59" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D59" s="5"/>
       <c r="T59" s="6"/>
     </row>
-    <row r="60" spans="4:20">
+    <row r="60" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D60" s="5"/>
       <c r="T60" s="6"/>
     </row>
-    <row r="61" spans="4:20">
+    <row r="61" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D61" s="5"/>
       <c r="T61" s="6"/>
     </row>
-    <row r="62" spans="4:20">
+    <row r="62" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D62" s="5"/>
       <c r="T62" s="6"/>
     </row>
-    <row r="63" spans="4:20">
+    <row r="63" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D63" s="5"/>
       <c r="T63" s="6"/>
     </row>
-    <row r="64" spans="4:20">
+    <row r="64" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D64" s="5"/>
       <c r="T64" s="6"/>
     </row>
-    <row r="65" spans="4:20">
+    <row r="65" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D65" s="5"/>
       <c r="T65" s="6"/>
     </row>
-    <row r="66" spans="4:20">
+    <row r="66" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D66" s="5"/>
       <c r="T66" s="6"/>
     </row>
-    <row r="67" spans="4:20">
+    <row r="67" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D67" s="5"/>
       <c r="T67" s="6"/>
     </row>
-    <row r="68" spans="4:20">
+    <row r="68" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D68" s="21"/>
       <c r="E68" s="22"/>
       <c r="F68" s="22"/>
@@ -4079,63 +4132,63 @@
       <c r="P68" s="22"/>
       <c r="T68" s="6"/>
     </row>
-    <row r="69" spans="4:20">
+    <row r="69" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D69" s="5"/>
       <c r="T69" s="6"/>
     </row>
-    <row r="70" spans="4:20">
+    <row r="70" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D70" s="5"/>
       <c r="T70" s="6"/>
     </row>
-    <row r="71" spans="4:20">
+    <row r="71" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D71" s="5"/>
       <c r="T71" s="6"/>
     </row>
-    <row r="72" spans="4:20">
+    <row r="72" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D72" s="5"/>
       <c r="T72" s="6"/>
     </row>
-    <row r="73" spans="4:20">
+    <row r="73" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D73" s="5"/>
       <c r="T73" s="6"/>
     </row>
-    <row r="74" spans="4:20">
+    <row r="74" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D74" s="5"/>
       <c r="T74" s="6"/>
     </row>
-    <row r="75" spans="4:20">
+    <row r="75" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D75" s="5"/>
       <c r="T75" s="6"/>
     </row>
-    <row r="76" spans="4:20">
+    <row r="76" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D76" s="5"/>
       <c r="T76" s="6"/>
     </row>
-    <row r="77" spans="4:20">
+    <row r="77" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D77" s="5"/>
       <c r="T77" s="6"/>
     </row>
-    <row r="78" spans="4:20">
+    <row r="78" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D78" s="5"/>
       <c r="T78" s="6"/>
     </row>
-    <row r="79" spans="4:20">
+    <row r="79" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D79" s="5"/>
       <c r="T79" s="6"/>
     </row>
-    <row r="80" spans="4:20">
+    <row r="80" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D80" s="5"/>
       <c r="T80" s="6"/>
     </row>
-    <row r="81" spans="4:20">
+    <row r="81" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D81" s="5"/>
       <c r="T81" s="6"/>
     </row>
-    <row r="82" spans="4:20">
+    <row r="82" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D82" s="5"/>
       <c r="T82" s="6"/>
     </row>
-    <row r="83" spans="4:20">
+    <row r="83" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D83" s="7"/>
       <c r="E83" s="8"/>
       <c r="F83" s="8"/>
@@ -4176,13 +4229,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3265C1DE-771B-466D-AFE8-2C836A595B59}">
   <dimension ref="B4:AJ81"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S4" sqref="S4"/>
+    <sheetView showGridLines="0" topLeftCell="A33" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AA73" sqref="AA73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="4" spans="2:36">
+    <row r="4" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B4" s="26" t="s">
         <v>17</v>
       </c>
@@ -4222,7 +4275,7 @@
       <c r="AI4" s="12"/>
       <c r="AJ4" s="13"/>
     </row>
-    <row r="5" spans="2:36">
+    <row r="5" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B5" s="14"/>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
@@ -4258,7 +4311,7 @@
       <c r="AI5" s="10"/>
       <c r="AJ5" s="15"/>
     </row>
-    <row r="6" spans="2:36">
+    <row r="6" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B6" s="14"/>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
@@ -4293,7 +4346,7 @@
       <c r="AI6" s="10"/>
       <c r="AJ6" s="15"/>
     </row>
-    <row r="7" spans="2:36">
+    <row r="7" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B7" s="14"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -4333,7 +4386,7 @@
       <c r="AI7" s="35"/>
       <c r="AJ7" s="15"/>
     </row>
-    <row r="8" spans="2:36">
+    <row r="8" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B8" s="14"/>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
@@ -4373,7 +4426,7 @@
       <c r="AI8" s="36"/>
       <c r="AJ8" s="15"/>
     </row>
-    <row r="9" spans="2:36">
+    <row r="9" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B9" s="14"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
@@ -4409,7 +4462,7 @@
       <c r="AI9" s="36"/>
       <c r="AJ9" s="15"/>
     </row>
-    <row r="10" spans="2:36" ht="18.75">
+    <row r="10" spans="2:36" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B10" s="14"/>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
@@ -4449,7 +4502,7 @@
       <c r="AI10" s="34"/>
       <c r="AJ10" s="15"/>
     </row>
-    <row r="11" spans="2:36">
+    <row r="11" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B11" s="14"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
@@ -4485,7 +4538,7 @@
       <c r="AI11" s="10"/>
       <c r="AJ11" s="15"/>
     </row>
-    <row r="12" spans="2:36">
+    <row r="12" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B12" s="14"/>
       <c r="C12" s="10"/>
       <c r="E12" s="10"/>
@@ -4520,7 +4573,7 @@
       <c r="AI12" s="10"/>
       <c r="AJ12" s="15"/>
     </row>
-    <row r="13" spans="2:36">
+    <row r="13" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B13" s="14"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
@@ -4556,7 +4609,7 @@
       <c r="AI13" s="10"/>
       <c r="AJ13" s="15"/>
     </row>
-    <row r="14" spans="2:36">
+    <row r="14" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B14" s="14"/>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
@@ -4592,7 +4645,7 @@
       <c r="AI14" s="10"/>
       <c r="AJ14" s="15"/>
     </row>
-    <row r="15" spans="2:36">
+    <row r="15" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B15" s="14"/>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
@@ -4628,7 +4681,7 @@
       <c r="AI15" s="10"/>
       <c r="AJ15" s="15"/>
     </row>
-    <row r="16" spans="2:36">
+    <row r="16" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B16" s="14"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
@@ -4664,7 +4717,7 @@
       <c r="AI16" s="10"/>
       <c r="AJ16" s="15"/>
     </row>
-    <row r="17" spans="2:36">
+    <row r="17" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B17" s="14"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
@@ -4700,7 +4753,7 @@
       <c r="AI17" s="10"/>
       <c r="AJ17" s="15"/>
     </row>
-    <row r="18" spans="2:36">
+    <row r="18" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B18" s="14"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
@@ -4736,7 +4789,7 @@
       <c r="AI18" s="10"/>
       <c r="AJ18" s="15"/>
     </row>
-    <row r="19" spans="2:36">
+    <row r="19" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B19" s="14"/>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
@@ -4772,7 +4825,7 @@
       <c r="AI19" s="10"/>
       <c r="AJ19" s="15"/>
     </row>
-    <row r="20" spans="2:36">
+    <row r="20" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B20" s="14"/>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
@@ -4808,7 +4861,7 @@
       <c r="AI20" s="10"/>
       <c r="AJ20" s="15"/>
     </row>
-    <row r="21" spans="2:36">
+    <row r="21" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B21" s="14"/>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
@@ -4844,7 +4897,7 @@
       <c r="AI21" s="10"/>
       <c r="AJ21" s="15"/>
     </row>
-    <row r="22" spans="2:36">
+    <row r="22" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B22" s="14"/>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
@@ -4880,7 +4933,7 @@
       <c r="AI22" s="10"/>
       <c r="AJ22" s="15"/>
     </row>
-    <row r="23" spans="2:36">
+    <row r="23" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B23" s="14"/>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
@@ -4915,7 +4968,7 @@
       <c r="AI23" s="10"/>
       <c r="AJ23" s="15"/>
     </row>
-    <row r="24" spans="2:36">
+    <row r="24" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B24" s="14"/>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
@@ -4951,7 +5004,7 @@
       <c r="AI24" s="10"/>
       <c r="AJ24" s="15"/>
     </row>
-    <row r="25" spans="2:36">
+    <row r="25" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B25" s="14"/>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
@@ -4986,7 +5039,7 @@
       <c r="AI25" s="10"/>
       <c r="AJ25" s="15"/>
     </row>
-    <row r="26" spans="2:36">
+    <row r="26" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B26" s="14"/>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
@@ -5022,7 +5075,7 @@
       <c r="AI26" s="10"/>
       <c r="AJ26" s="15"/>
     </row>
-    <row r="27" spans="2:36">
+    <row r="27" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B27" s="14"/>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
@@ -5058,7 +5111,7 @@
       <c r="AI27" s="10"/>
       <c r="AJ27" s="15"/>
     </row>
-    <row r="28" spans="2:36">
+    <row r="28" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B28" s="14"/>
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
@@ -5094,7 +5147,7 @@
       <c r="AI28" s="10"/>
       <c r="AJ28" s="15"/>
     </row>
-    <row r="29" spans="2:36">
+    <row r="29" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B29" s="14"/>
       <c r="C29" s="10"/>
       <c r="D29" s="10"/>
@@ -5130,7 +5183,7 @@
       <c r="AI29" s="10"/>
       <c r="AJ29" s="15"/>
     </row>
-    <row r="30" spans="2:36">
+    <row r="30" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B30" s="14"/>
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
@@ -5166,7 +5219,7 @@
       <c r="AI30" s="10"/>
       <c r="AJ30" s="15"/>
     </row>
-    <row r="31" spans="2:36">
+    <row r="31" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B31" s="14"/>
       <c r="C31" s="10"/>
       <c r="D31" s="10"/>
@@ -5202,7 +5255,7 @@
       <c r="AI31" s="10"/>
       <c r="AJ31" s="15"/>
     </row>
-    <row r="32" spans="2:36">
+    <row r="32" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B32" s="14"/>
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
@@ -5238,7 +5291,7 @@
       <c r="AI32" s="10"/>
       <c r="AJ32" s="15"/>
     </row>
-    <row r="33" spans="2:36">
+    <row r="33" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B33" s="14"/>
       <c r="C33" s="10"/>
       <c r="D33" s="10"/>
@@ -5274,7 +5327,7 @@
       <c r="AI33" s="10"/>
       <c r="AJ33" s="15"/>
     </row>
-    <row r="34" spans="2:36">
+    <row r="34" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B34" s="14"/>
       <c r="C34" s="10"/>
       <c r="D34" s="10"/>
@@ -5310,7 +5363,7 @@
       <c r="AI34" s="10"/>
       <c r="AJ34" s="15"/>
     </row>
-    <row r="35" spans="2:36">
+    <row r="35" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B35" s="14"/>
       <c r="C35" s="10"/>
       <c r="D35" s="10"/>
@@ -5346,7 +5399,7 @@
       <c r="AI35" s="10"/>
       <c r="AJ35" s="15"/>
     </row>
-    <row r="36" spans="2:36">
+    <row r="36" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B36" s="14"/>
       <c r="C36" s="10"/>
       <c r="D36" s="10"/>
@@ -5382,7 +5435,7 @@
       <c r="AI36" s="10"/>
       <c r="AJ36" s="15"/>
     </row>
-    <row r="37" spans="2:36">
+    <row r="37" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B37" s="14"/>
       <c r="C37" s="10"/>
       <c r="D37" s="10"/>
@@ -5418,7 +5471,7 @@
       <c r="AI37" s="10"/>
       <c r="AJ37" s="15"/>
     </row>
-    <row r="38" spans="2:36">
+    <row r="38" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B38" s="14"/>
       <c r="C38" s="10"/>
       <c r="D38" s="10"/>
@@ -5454,7 +5507,7 @@
       <c r="AI38" s="10"/>
       <c r="AJ38" s="15"/>
     </row>
-    <row r="39" spans="2:36">
+    <row r="39" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B39" s="14"/>
       <c r="C39" s="10"/>
       <c r="D39" s="10"/>
@@ -5490,7 +5543,7 @@
       <c r="AI39" s="10"/>
       <c r="AJ39" s="15"/>
     </row>
-    <row r="40" spans="2:36">
+    <row r="40" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B40" s="14"/>
       <c r="C40" s="10"/>
       <c r="D40" s="10"/>
@@ -5526,7 +5579,7 @@
       <c r="AI40" s="10"/>
       <c r="AJ40" s="15"/>
     </row>
-    <row r="41" spans="2:36">
+    <row r="41" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B41" s="16"/>
       <c r="C41" s="17"/>
       <c r="D41" s="17"/>
@@ -5562,7 +5615,7 @@
       <c r="AI41" s="17"/>
       <c r="AJ41" s="18"/>
     </row>
-    <row r="44" spans="2:36">
+    <row r="44" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B44" s="26" t="s">
         <v>14</v>
       </c>
@@ -5583,7 +5636,7 @@
       <c r="Q44" s="12"/>
       <c r="R44" s="13"/>
     </row>
-    <row r="45" spans="2:36">
+    <row r="45" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B45" s="14"/>
       <c r="C45" s="10"/>
       <c r="D45" s="10"/>
@@ -5602,7 +5655,7 @@
       <c r="Q45" s="10"/>
       <c r="R45" s="15"/>
     </row>
-    <row r="46" spans="2:36">
+    <row r="46" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B46" s="14"/>
       <c r="C46" s="10"/>
       <c r="D46" s="10"/>
@@ -5621,7 +5674,7 @@
       <c r="Q46" s="10"/>
       <c r="R46" s="15"/>
     </row>
-    <row r="47" spans="2:36">
+    <row r="47" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B47" s="14"/>
       <c r="C47" s="10"/>
       <c r="D47" s="10"/>
@@ -5642,7 +5695,7 @@
       <c r="Q47" s="35"/>
       <c r="R47" s="15"/>
     </row>
-    <row r="48" spans="2:36">
+    <row r="48" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B48" s="14"/>
       <c r="C48" s="10"/>
       <c r="D48" s="10"/>
@@ -5663,7 +5716,7 @@
       <c r="Q48" s="36"/>
       <c r="R48" s="15"/>
     </row>
-    <row r="49" spans="2:18">
+    <row r="49" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B49" s="14"/>
       <c r="C49" s="10"/>
       <c r="D49" s="10"/>
@@ -5682,7 +5735,7 @@
       <c r="Q49" s="36"/>
       <c r="R49" s="15"/>
     </row>
-    <row r="50" spans="2:18" ht="18.75">
+    <row r="50" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B50" s="14"/>
       <c r="C50" s="10"/>
       <c r="D50" s="10"/>
@@ -5702,7 +5755,7 @@
       <c r="Q50" s="34"/>
       <c r="R50" s="15"/>
     </row>
-    <row r="51" spans="2:18">
+    <row r="51" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B51" s="14"/>
       <c r="C51" s="10"/>
       <c r="D51" s="10"/>
@@ -5721,7 +5774,7 @@
       <c r="Q51" s="10"/>
       <c r="R51" s="15"/>
     </row>
-    <row r="52" spans="2:18">
+    <row r="52" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B52" s="14"/>
       <c r="C52" s="10"/>
       <c r="D52" s="10"/>
@@ -5740,7 +5793,7 @@
       <c r="Q52" s="10"/>
       <c r="R52" s="15"/>
     </row>
-    <row r="53" spans="2:18">
+    <row r="53" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B53" s="14"/>
       <c r="C53" s="10"/>
       <c r="D53" s="10"/>
@@ -5759,7 +5812,7 @@
       <c r="Q53" s="10"/>
       <c r="R53" s="15"/>
     </row>
-    <row r="54" spans="2:18">
+    <row r="54" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B54" s="14"/>
       <c r="C54" s="10"/>
       <c r="D54" s="10"/>
@@ -5778,7 +5831,7 @@
       <c r="Q54" s="10"/>
       <c r="R54" s="15"/>
     </row>
-    <row r="55" spans="2:18">
+    <row r="55" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B55" s="14"/>
       <c r="C55" s="10"/>
       <c r="D55" s="10"/>
@@ -5797,7 +5850,7 @@
       <c r="Q55" s="10"/>
       <c r="R55" s="15"/>
     </row>
-    <row r="56" spans="2:18">
+    <row r="56" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B56" s="14"/>
       <c r="C56" s="10"/>
       <c r="D56" s="10"/>
@@ -5816,7 +5869,7 @@
       <c r="Q56" s="10"/>
       <c r="R56" s="15"/>
     </row>
-    <row r="57" spans="2:18">
+    <row r="57" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B57" s="14"/>
       <c r="C57" s="10"/>
       <c r="D57" s="10"/>
@@ -5835,7 +5888,7 @@
       <c r="Q57" s="10"/>
       <c r="R57" s="15"/>
     </row>
-    <row r="58" spans="2:18">
+    <row r="58" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B58" s="14"/>
       <c r="C58" s="10"/>
       <c r="D58" s="10"/>
@@ -5854,7 +5907,7 @@
       <c r="Q58" s="10"/>
       <c r="R58" s="15"/>
     </row>
-    <row r="59" spans="2:18">
+    <row r="59" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B59" s="14"/>
       <c r="C59" s="10"/>
       <c r="D59" s="10"/>
@@ -5873,7 +5926,7 @@
       <c r="Q59" s="10"/>
       <c r="R59" s="15"/>
     </row>
-    <row r="60" spans="2:18">
+    <row r="60" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B60" s="14"/>
       <c r="C60" s="10"/>
       <c r="D60" s="10"/>
@@ -5892,7 +5945,7 @@
       <c r="Q60" s="10"/>
       <c r="R60" s="15"/>
     </row>
-    <row r="61" spans="2:18">
+    <row r="61" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B61" s="14"/>
       <c r="C61" s="10"/>
       <c r="D61" s="10"/>
@@ -5911,7 +5964,7 @@
       <c r="Q61" s="10"/>
       <c r="R61" s="15"/>
     </row>
-    <row r="62" spans="2:18">
+    <row r="62" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B62" s="14"/>
       <c r="C62" s="10"/>
       <c r="D62" s="10"/>
@@ -5930,7 +5983,7 @@
       <c r="Q62" s="10"/>
       <c r="R62" s="15"/>
     </row>
-    <row r="63" spans="2:18">
+    <row r="63" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B63" s="14"/>
       <c r="C63" s="10"/>
       <c r="D63" s="10"/>
@@ -5949,7 +6002,7 @@
       <c r="Q63" s="10"/>
       <c r="R63" s="15"/>
     </row>
-    <row r="64" spans="2:18">
+    <row r="64" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B64" s="14"/>
       <c r="C64" s="10"/>
       <c r="D64" s="10"/>
@@ -5967,7 +6020,7 @@
       <c r="Q64" s="10"/>
       <c r="R64" s="15"/>
     </row>
-    <row r="65" spans="2:18">
+    <row r="65" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B65" s="14"/>
       <c r="C65" s="10"/>
       <c r="D65" s="10"/>
@@ -5986,7 +6039,7 @@
       <c r="Q65" s="10"/>
       <c r="R65" s="15"/>
     </row>
-    <row r="66" spans="2:18">
+    <row r="66" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B66" s="14"/>
       <c r="C66" s="10"/>
       <c r="D66" s="10"/>
@@ -6005,7 +6058,7 @@
       <c r="Q66" s="10"/>
       <c r="R66" s="15"/>
     </row>
-    <row r="67" spans="2:18">
+    <row r="67" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B67" s="14"/>
       <c r="C67" s="10"/>
       <c r="D67" s="10"/>
@@ -6024,7 +6077,7 @@
       <c r="Q67" s="10"/>
       <c r="R67" s="15"/>
     </row>
-    <row r="68" spans="2:18">
+    <row r="68" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B68" s="14"/>
       <c r="C68" s="10"/>
       <c r="D68" s="10"/>
@@ -6043,7 +6096,7 @@
       <c r="Q68" s="10"/>
       <c r="R68" s="15"/>
     </row>
-    <row r="69" spans="2:18">
+    <row r="69" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B69" s="14"/>
       <c r="C69" s="10"/>
       <c r="D69" s="10"/>
@@ -6062,7 +6115,7 @@
       <c r="Q69" s="10"/>
       <c r="R69" s="15"/>
     </row>
-    <row r="70" spans="2:18">
+    <row r="70" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B70" s="14"/>
       <c r="C70" s="10"/>
       <c r="D70" s="10"/>
@@ -6081,7 +6134,7 @@
       <c r="Q70" s="10"/>
       <c r="R70" s="15"/>
     </row>
-    <row r="71" spans="2:18">
+    <row r="71" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B71" s="14"/>
       <c r="C71" s="10"/>
       <c r="D71" s="10"/>
@@ -6100,7 +6153,7 @@
       <c r="Q71" s="10"/>
       <c r="R71" s="15"/>
     </row>
-    <row r="72" spans="2:18">
+    <row r="72" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B72" s="14"/>
       <c r="C72" s="10"/>
       <c r="D72" s="10"/>
@@ -6119,7 +6172,7 @@
       <c r="Q72" s="10"/>
       <c r="R72" s="15"/>
     </row>
-    <row r="73" spans="2:18">
+    <row r="73" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B73" s="14"/>
       <c r="C73" s="10"/>
       <c r="D73" s="10"/>
@@ -6138,7 +6191,7 @@
       <c r="Q73" s="10"/>
       <c r="R73" s="15"/>
     </row>
-    <row r="74" spans="2:18">
+    <row r="74" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B74" s="14"/>
       <c r="C74" s="10"/>
       <c r="D74" s="10"/>
@@ -6157,7 +6210,7 @@
       <c r="Q74" s="10"/>
       <c r="R74" s="15"/>
     </row>
-    <row r="75" spans="2:18">
+    <row r="75" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B75" s="14"/>
       <c r="C75" s="10"/>
       <c r="D75" s="10"/>
@@ -6176,7 +6229,7 @@
       <c r="Q75" s="10"/>
       <c r="R75" s="15"/>
     </row>
-    <row r="76" spans="2:18">
+    <row r="76" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B76" s="14"/>
       <c r="C76" s="10"/>
       <c r="D76" s="10"/>
@@ -6195,7 +6248,7 @@
       <c r="Q76" s="10"/>
       <c r="R76" s="15"/>
     </row>
-    <row r="77" spans="2:18">
+    <row r="77" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B77" s="14"/>
       <c r="C77" s="10"/>
       <c r="D77" s="10"/>
@@ -6214,7 +6267,7 @@
       <c r="Q77" s="10"/>
       <c r="R77" s="15"/>
     </row>
-    <row r="78" spans="2:18">
+    <row r="78" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B78" s="14"/>
       <c r="C78" s="10"/>
       <c r="D78" s="10"/>
@@ -6233,7 +6286,7 @@
       <c r="Q78" s="10"/>
       <c r="R78" s="15"/>
     </row>
-    <row r="79" spans="2:18">
+    <row r="79" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B79" s="14"/>
       <c r="C79" s="10"/>
       <c r="D79" s="10"/>
@@ -6252,7 +6305,7 @@
       <c r="Q79" s="10"/>
       <c r="R79" s="15"/>
     </row>
-    <row r="80" spans="2:18">
+    <row r="80" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B80" s="14"/>
       <c r="C80" s="10"/>
       <c r="D80" s="10"/>
@@ -6271,7 +6324,7 @@
       <c r="Q80" s="10"/>
       <c r="R80" s="15"/>
     </row>
-    <row r="81" spans="2:18">
+    <row r="81" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B81" s="16"/>
       <c r="C81" s="17"/>
       <c r="D81" s="17"/>
@@ -6311,16 +6364,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{800CFA05-9B27-4650-A169-A5D3EBB0D79D}">
   <dimension ref="B2:AJ79"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="AJ17" sqref="AJ17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:36">
+    <row r="2" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B2" s="26" t="s">
         <v>18</v>
       </c>
@@ -6361,7 +6414,7 @@
       <c r="AI2" s="12"/>
       <c r="AJ2" s="13"/>
     </row>
-    <row r="3" spans="2:36">
+    <row r="3" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B3" s="14"/>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
@@ -6398,7 +6451,7 @@
       <c r="AI3" s="10"/>
       <c r="AJ3" s="15"/>
     </row>
-    <row r="4" spans="2:36">
+    <row r="4" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B4" s="14"/>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -6435,7 +6488,7 @@
       <c r="AI4" s="10"/>
       <c r="AJ4" s="15"/>
     </row>
-    <row r="5" spans="2:36">
+    <row r="5" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B5" s="14"/>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
@@ -6476,7 +6529,7 @@
       <c r="AI5" s="35"/>
       <c r="AJ5" s="15"/>
     </row>
-    <row r="6" spans="2:36">
+    <row r="6" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B6" s="14"/>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
@@ -6517,7 +6570,7 @@
       <c r="AI6" s="36"/>
       <c r="AJ6" s="15"/>
     </row>
-    <row r="7" spans="2:36">
+    <row r="7" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B7" s="14"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -6554,7 +6607,7 @@
       <c r="AI7" s="36"/>
       <c r="AJ7" s="15"/>
     </row>
-    <row r="8" spans="2:36" ht="18.75">
+    <row r="8" spans="2:36" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B8" s="14"/>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
@@ -6595,7 +6648,7 @@
       <c r="AI8" s="34"/>
       <c r="AJ8" s="15"/>
     </row>
-    <row r="9" spans="2:36">
+    <row r="9" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B9" s="14"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
@@ -6632,7 +6685,7 @@
       <c r="AI9" s="10"/>
       <c r="AJ9" s="15"/>
     </row>
-    <row r="10" spans="2:36">
+    <row r="10" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B10" s="14"/>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
@@ -6669,7 +6722,7 @@
       <c r="AI10" s="10"/>
       <c r="AJ10" s="15"/>
     </row>
-    <row r="11" spans="2:36">
+    <row r="11" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B11" s="14"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
@@ -6706,7 +6759,7 @@
       <c r="AI11" s="10"/>
       <c r="AJ11" s="15"/>
     </row>
-    <row r="12" spans="2:36">
+    <row r="12" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B12" s="14"/>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
@@ -6743,7 +6796,7 @@
       <c r="AI12" s="10"/>
       <c r="AJ12" s="15"/>
     </row>
-    <row r="13" spans="2:36">
+    <row r="13" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B13" s="14"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
@@ -6780,7 +6833,7 @@
       <c r="AI13" s="10"/>
       <c r="AJ13" s="15"/>
     </row>
-    <row r="14" spans="2:36">
+    <row r="14" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B14" s="14"/>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
@@ -6817,7 +6870,7 @@
       <c r="AI14" s="10"/>
       <c r="AJ14" s="15"/>
     </row>
-    <row r="15" spans="2:36">
+    <row r="15" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B15" s="14"/>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
@@ -6854,7 +6907,7 @@
       <c r="AI15" s="10"/>
       <c r="AJ15" s="15"/>
     </row>
-    <row r="16" spans="2:36">
+    <row r="16" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B16" s="14"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
@@ -6891,7 +6944,7 @@
       <c r="AI16" s="10"/>
       <c r="AJ16" s="15"/>
     </row>
-    <row r="17" spans="2:36">
+    <row r="17" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B17" s="14"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
@@ -6930,7 +6983,7 @@
       <c r="AI17" s="10"/>
       <c r="AJ17" s="15"/>
     </row>
-    <row r="18" spans="2:36">
+    <row r="18" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B18" s="14"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
@@ -6967,7 +7020,7 @@
       <c r="AI18" s="10"/>
       <c r="AJ18" s="15"/>
     </row>
-    <row r="19" spans="2:36">
+    <row r="19" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B19" s="14"/>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
@@ -7004,7 +7057,7 @@
       <c r="AI19" s="10"/>
       <c r="AJ19" s="15"/>
     </row>
-    <row r="20" spans="2:36">
+    <row r="20" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B20" s="14"/>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
@@ -7041,7 +7094,7 @@
       <c r="AI20" s="10"/>
       <c r="AJ20" s="15"/>
     </row>
-    <row r="21" spans="2:36">
+    <row r="21" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B21" s="14"/>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
@@ -7078,7 +7131,7 @@
       <c r="AI21" s="10"/>
       <c r="AJ21" s="15"/>
     </row>
-    <row r="22" spans="2:36">
+    <row r="22" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B22" s="14"/>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
@@ -7115,7 +7168,7 @@
       <c r="AI22" s="10"/>
       <c r="AJ22" s="15"/>
     </row>
-    <row r="23" spans="2:36">
+    <row r="23" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B23" s="14"/>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
@@ -7152,7 +7205,7 @@
       <c r="AI23" s="10"/>
       <c r="AJ23" s="15"/>
     </row>
-    <row r="24" spans="2:36">
+    <row r="24" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B24" s="14"/>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
@@ -7189,7 +7242,7 @@
       <c r="AI24" s="10"/>
       <c r="AJ24" s="15"/>
     </row>
-    <row r="25" spans="2:36">
+    <row r="25" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B25" s="14"/>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
@@ -7226,7 +7279,7 @@
       <c r="AI25" s="10"/>
       <c r="AJ25" s="15"/>
     </row>
-    <row r="26" spans="2:36">
+    <row r="26" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B26" s="14"/>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
@@ -7263,7 +7316,7 @@
       <c r="AI26" s="10"/>
       <c r="AJ26" s="15"/>
     </row>
-    <row r="27" spans="2:36">
+    <row r="27" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B27" s="14"/>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
@@ -7300,7 +7353,7 @@
       <c r="AI27" s="10"/>
       <c r="AJ27" s="15"/>
     </row>
-    <row r="28" spans="2:36">
+    <row r="28" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B28" s="14"/>
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
@@ -7337,7 +7390,7 @@
       <c r="AI28" s="10"/>
       <c r="AJ28" s="15"/>
     </row>
-    <row r="29" spans="2:36">
+    <row r="29" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B29" s="14"/>
       <c r="C29" s="10"/>
       <c r="D29" s="10"/>
@@ -7374,7 +7427,7 @@
       <c r="AI29" s="10"/>
       <c r="AJ29" s="15"/>
     </row>
-    <row r="30" spans="2:36">
+    <row r="30" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B30" s="14"/>
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
@@ -7411,7 +7464,7 @@
       <c r="AI30" s="10"/>
       <c r="AJ30" s="15"/>
     </row>
-    <row r="31" spans="2:36">
+    <row r="31" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B31" s="14"/>
       <c r="C31" s="10"/>
       <c r="D31" s="10"/>
@@ -7448,7 +7501,7 @@
       <c r="AI31" s="10"/>
       <c r="AJ31" s="15"/>
     </row>
-    <row r="32" spans="2:36">
+    <row r="32" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B32" s="14"/>
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
@@ -7485,7 +7538,7 @@
       <c r="AI32" s="10"/>
       <c r="AJ32" s="15"/>
     </row>
-    <row r="33" spans="2:36">
+    <row r="33" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B33" s="14"/>
       <c r="C33" s="10"/>
       <c r="D33" s="10"/>
@@ -7522,7 +7575,7 @@
       <c r="AI33" s="10"/>
       <c r="AJ33" s="15"/>
     </row>
-    <row r="34" spans="2:36">
+    <row r="34" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B34" s="14"/>
       <c r="C34" s="10"/>
       <c r="D34" s="10"/>
@@ -7559,7 +7612,7 @@
       <c r="AI34" s="10"/>
       <c r="AJ34" s="15"/>
     </row>
-    <row r="35" spans="2:36">
+    <row r="35" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B35" s="14"/>
       <c r="C35" s="10"/>
       <c r="D35" s="10"/>
@@ -7596,7 +7649,7 @@
       <c r="AI35" s="10"/>
       <c r="AJ35" s="15"/>
     </row>
-    <row r="36" spans="2:36">
+    <row r="36" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B36" s="14"/>
       <c r="C36" s="10"/>
       <c r="D36" s="10"/>
@@ -7633,7 +7686,7 @@
       <c r="AI36" s="10"/>
       <c r="AJ36" s="15"/>
     </row>
-    <row r="37" spans="2:36">
+    <row r="37" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B37" s="14"/>
       <c r="C37" s="10"/>
       <c r="D37" s="10"/>
@@ -7670,7 +7723,7 @@
       <c r="AI37" s="10"/>
       <c r="AJ37" s="15"/>
     </row>
-    <row r="38" spans="2:36">
+    <row r="38" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B38" s="14"/>
       <c r="C38" s="10"/>
       <c r="D38" s="10"/>
@@ -7707,7 +7760,7 @@
       <c r="AI38" s="10"/>
       <c r="AJ38" s="15"/>
     </row>
-    <row r="39" spans="2:36">
+    <row r="39" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B39" s="16"/>
       <c r="C39" s="17"/>
       <c r="D39" s="17"/>
@@ -7744,7 +7797,7 @@
       <c r="AI39" s="17"/>
       <c r="AJ39" s="18"/>
     </row>
-    <row r="40" spans="2:36">
+    <row r="40" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B40"/>
       <c r="C40"/>
       <c r="D40"/>
@@ -7781,7 +7834,7 @@
       <c r="AI40"/>
       <c r="AJ40"/>
     </row>
-    <row r="41" spans="2:36">
+    <row r="41" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B41"/>
       <c r="C41"/>
       <c r="D41"/>
@@ -7818,7 +7871,7 @@
       <c r="AI41"/>
       <c r="AJ41"/>
     </row>
-    <row r="42" spans="2:36">
+    <row r="42" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B42" s="11"/>
       <c r="C42" s="12"/>
       <c r="D42" s="12"/>
@@ -7855,7 +7908,7 @@
       <c r="AI42"/>
       <c r="AJ42"/>
     </row>
-    <row r="43" spans="2:36">
+    <row r="43" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B43" s="14"/>
       <c r="C43" s="10"/>
       <c r="D43" s="10"/>
@@ -7892,7 +7945,7 @@
       <c r="AI43"/>
       <c r="AJ43"/>
     </row>
-    <row r="44" spans="2:36">
+    <row r="44" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B44" s="14"/>
       <c r="C44" s="10"/>
       <c r="D44" s="10"/>
@@ -7929,7 +7982,7 @@
       <c r="AI44"/>
       <c r="AJ44"/>
     </row>
-    <row r="45" spans="2:36">
+    <row r="45" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B45" s="14"/>
       <c r="C45" s="10"/>
       <c r="D45" s="10"/>
@@ -7968,7 +8021,7 @@
       <c r="AI45"/>
       <c r="AJ45"/>
     </row>
-    <row r="46" spans="2:36">
+    <row r="46" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B46" s="14"/>
       <c r="C46" s="10"/>
       <c r="D46" s="10"/>
@@ -8007,7 +8060,7 @@
       <c r="AI46"/>
       <c r="AJ46"/>
     </row>
-    <row r="47" spans="2:36">
+    <row r="47" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B47" s="14"/>
       <c r="C47" s="10"/>
       <c r="D47" s="10"/>
@@ -8044,7 +8097,7 @@
       <c r="AI47"/>
       <c r="AJ47"/>
     </row>
-    <row r="48" spans="2:36" ht="18.75">
+    <row r="48" spans="2:36" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B48" s="14"/>
       <c r="C48" s="10"/>
       <c r="D48" s="10"/>
@@ -8083,7 +8136,7 @@
       <c r="AI48"/>
       <c r="AJ48"/>
     </row>
-    <row r="49" spans="2:36">
+    <row r="49" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B49" s="14"/>
       <c r="C49" s="10"/>
       <c r="D49" s="10"/>
@@ -8120,7 +8173,7 @@
       <c r="AI49"/>
       <c r="AJ49"/>
     </row>
-    <row r="50" spans="2:36">
+    <row r="50" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B50" s="14"/>
       <c r="C50" s="10"/>
       <c r="D50" s="10"/>
@@ -8157,7 +8210,7 @@
       <c r="AI50"/>
       <c r="AJ50"/>
     </row>
-    <row r="51" spans="2:36">
+    <row r="51" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B51" s="14"/>
       <c r="C51" s="10"/>
       <c r="D51" s="10"/>
@@ -8194,7 +8247,7 @@
       <c r="AI51"/>
       <c r="AJ51"/>
     </row>
-    <row r="52" spans="2:36">
+    <row r="52" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B52" s="14"/>
       <c r="C52" s="10"/>
       <c r="D52" s="10"/>
@@ -8231,7 +8284,7 @@
       <c r="AI52"/>
       <c r="AJ52"/>
     </row>
-    <row r="53" spans="2:36">
+    <row r="53" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B53" s="14"/>
       <c r="C53" s="10"/>
       <c r="D53" s="10"/>
@@ -8268,7 +8321,7 @@
       <c r="AI53"/>
       <c r="AJ53"/>
     </row>
-    <row r="54" spans="2:36">
+    <row r="54" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B54" s="14"/>
       <c r="C54" s="10"/>
       <c r="D54" s="10"/>
@@ -8305,7 +8358,7 @@
       <c r="AI54"/>
       <c r="AJ54"/>
     </row>
-    <row r="55" spans="2:36">
+    <row r="55" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B55" s="14"/>
       <c r="C55" s="10"/>
       <c r="D55" s="10"/>
@@ -8342,7 +8395,7 @@
       <c r="AI55"/>
       <c r="AJ55"/>
     </row>
-    <row r="56" spans="2:36">
+    <row r="56" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B56" s="14"/>
       <c r="C56" s="10"/>
       <c r="D56" s="10"/>
@@ -8379,7 +8432,7 @@
       <c r="AI56"/>
       <c r="AJ56"/>
     </row>
-    <row r="57" spans="2:36">
+    <row r="57" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B57" s="14"/>
       <c r="C57" s="10"/>
       <c r="D57" s="10"/>
@@ -8416,7 +8469,7 @@
       <c r="AI57"/>
       <c r="AJ57"/>
     </row>
-    <row r="58" spans="2:36">
+    <row r="58" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B58" s="14"/>
       <c r="C58" s="10"/>
       <c r="D58" s="10"/>
@@ -8455,7 +8508,7 @@
       <c r="AI58"/>
       <c r="AJ58"/>
     </row>
-    <row r="59" spans="2:36">
+    <row r="59" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B59" s="14"/>
       <c r="C59" s="10"/>
       <c r="D59" s="10"/>
@@ -8492,7 +8545,7 @@
       <c r="AI59"/>
       <c r="AJ59"/>
     </row>
-    <row r="60" spans="2:36">
+    <row r="60" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B60" s="14"/>
       <c r="C60" s="10"/>
       <c r="D60" s="10"/>
@@ -8529,7 +8582,7 @@
       <c r="AI60"/>
       <c r="AJ60"/>
     </row>
-    <row r="61" spans="2:36">
+    <row r="61" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B61" s="14"/>
       <c r="C61" s="10"/>
       <c r="D61" s="10"/>
@@ -8566,7 +8619,7 @@
       <c r="AI61"/>
       <c r="AJ61"/>
     </row>
-    <row r="62" spans="2:36">
+    <row r="62" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B62" s="14"/>
       <c r="C62" s="10"/>
       <c r="D62" s="10"/>
@@ -8603,7 +8656,7 @@
       <c r="AI62"/>
       <c r="AJ62"/>
     </row>
-    <row r="63" spans="2:36">
+    <row r="63" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B63" s="14"/>
       <c r="C63" s="10"/>
       <c r="D63" s="10"/>
@@ -8640,7 +8693,7 @@
       <c r="AI63"/>
       <c r="AJ63"/>
     </row>
-    <row r="64" spans="2:36">
+    <row r="64" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B64" s="14"/>
       <c r="C64" s="10"/>
       <c r="D64" s="10"/>
@@ -8677,7 +8730,7 @@
       <c r="AI64"/>
       <c r="AJ64"/>
     </row>
-    <row r="65" spans="2:36">
+    <row r="65" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B65" s="14"/>
       <c r="C65" s="10"/>
       <c r="D65" s="10"/>
@@ -8714,7 +8767,7 @@
       <c r="AI65"/>
       <c r="AJ65"/>
     </row>
-    <row r="66" spans="2:36">
+    <row r="66" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B66" s="14"/>
       <c r="C66" s="10"/>
       <c r="D66" s="10"/>
@@ -8751,7 +8804,7 @@
       <c r="AI66"/>
       <c r="AJ66"/>
     </row>
-    <row r="67" spans="2:36">
+    <row r="67" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B67" s="14"/>
       <c r="C67" s="10"/>
       <c r="D67" s="10"/>
@@ -8788,7 +8841,7 @@
       <c r="AI67"/>
       <c r="AJ67"/>
     </row>
-    <row r="68" spans="2:36">
+    <row r="68" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B68" s="14"/>
       <c r="C68" s="10"/>
       <c r="D68" s="10"/>
@@ -8825,7 +8878,7 @@
       <c r="AI68"/>
       <c r="AJ68"/>
     </row>
-    <row r="69" spans="2:36">
+    <row r="69" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B69" s="14"/>
       <c r="C69" s="10"/>
       <c r="D69" s="10"/>
@@ -8862,7 +8915,7 @@
       <c r="AI69"/>
       <c r="AJ69"/>
     </row>
-    <row r="70" spans="2:36">
+    <row r="70" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B70" s="14"/>
       <c r="C70" s="10"/>
       <c r="D70" s="10"/>
@@ -8899,7 +8952,7 @@
       <c r="AI70"/>
       <c r="AJ70"/>
     </row>
-    <row r="71" spans="2:36">
+    <row r="71" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B71" s="14"/>
       <c r="C71" s="10"/>
       <c r="D71" s="10"/>
@@ -8936,7 +8989,7 @@
       <c r="AI71"/>
       <c r="AJ71"/>
     </row>
-    <row r="72" spans="2:36">
+    <row r="72" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B72" s="14"/>
       <c r="C72" s="10"/>
       <c r="D72" s="10"/>
@@ -8973,7 +9026,7 @@
       <c r="AI72"/>
       <c r="AJ72"/>
     </row>
-    <row r="73" spans="2:36">
+    <row r="73" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B73" s="14"/>
       <c r="C73" s="10"/>
       <c r="D73" s="10"/>
@@ -9010,7 +9063,7 @@
       <c r="AI73"/>
       <c r="AJ73"/>
     </row>
-    <row r="74" spans="2:36">
+    <row r="74" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B74" s="14"/>
       <c r="C74" s="10"/>
       <c r="D74" s="10"/>
@@ -9047,7 +9100,7 @@
       <c r="AI74"/>
       <c r="AJ74"/>
     </row>
-    <row r="75" spans="2:36">
+    <row r="75" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B75" s="14"/>
       <c r="C75" s="10"/>
       <c r="D75" s="10"/>
@@ -9084,7 +9137,7 @@
       <c r="AI75"/>
       <c r="AJ75"/>
     </row>
-    <row r="76" spans="2:36">
+    <row r="76" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B76" s="14"/>
       <c r="C76" s="10"/>
       <c r="D76" s="10"/>
@@ -9121,7 +9174,7 @@
       <c r="AI76"/>
       <c r="AJ76"/>
     </row>
-    <row r="77" spans="2:36">
+    <row r="77" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B77" s="14"/>
       <c r="C77" s="10"/>
       <c r="D77" s="10"/>
@@ -9158,7 +9211,7 @@
       <c r="AI77"/>
       <c r="AJ77"/>
     </row>
-    <row r="78" spans="2:36">
+    <row r="78" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B78" s="14"/>
       <c r="C78" s="10"/>
       <c r="D78" s="10"/>
@@ -9195,7 +9248,7 @@
       <c r="AI78"/>
       <c r="AJ78"/>
     </row>
-    <row r="79" spans="2:36">
+    <row r="79" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B79" s="16"/>
       <c r="C79" s="17"/>
       <c r="D79" s="17"/>
@@ -9258,7 +9311,7 @@
       <selection activeCell="AN34" sqref="AN34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -9269,13 +9322,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7155BC64-C482-45D1-904B-A1912B1B7F57}">
   <dimension ref="B3:AJ89"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AF43" sqref="AF43"/>
+    <sheetView showGridLines="0" topLeftCell="A24" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AG15" sqref="AG15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="2:36" ht="15.75">
+    <row r="3" spans="2:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="11"/>
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
@@ -9313,7 +9366,7 @@
       <c r="AI3" s="12"/>
       <c r="AJ3" s="13"/>
     </row>
-    <row r="4" spans="2:36">
+    <row r="4" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B4" s="14"/>
       <c r="C4" s="10"/>
       <c r="D4" s="24" t="s">
@@ -9351,7 +9404,7 @@
       <c r="AI4" s="10"/>
       <c r="AJ4" s="15"/>
     </row>
-    <row r="5" spans="2:36">
+    <row r="5" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B5" s="14"/>
       <c r="C5" s="10"/>
       <c r="E5" s="10"/>
@@ -9386,7 +9439,7 @@
       <c r="AI5" s="10"/>
       <c r="AJ5" s="15"/>
     </row>
-    <row r="6" spans="2:36">
+    <row r="6" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B6" s="14"/>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
@@ -9401,10 +9454,10 @@
       <c r="M6" s="10"/>
       <c r="N6" s="10"/>
       <c r="O6" s="10"/>
-      <c r="P6" s="37" t="s">
+      <c r="P6" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="Q6" s="37"/>
+      <c r="Q6" s="38"/>
       <c r="R6" s="15"/>
       <c r="T6" s="14"/>
       <c r="U6" s="10"/>
@@ -9419,13 +9472,13 @@
       <c r="AE6" s="10"/>
       <c r="AF6" s="10"/>
       <c r="AG6" s="10"/>
-      <c r="AH6" s="37" t="s">
+      <c r="AH6" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="AI6" s="37"/>
+      <c r="AI6" s="38"/>
       <c r="AJ6" s="15"/>
     </row>
-    <row r="7" spans="2:36">
+    <row r="7" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B7" s="14"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -9465,7 +9518,7 @@
       <c r="AI7" s="36"/>
       <c r="AJ7" s="15"/>
     </row>
-    <row r="8" spans="2:36">
+    <row r="8" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B8" s="14"/>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
@@ -9501,7 +9554,7 @@
       <c r="AI8" s="36"/>
       <c r="AJ8" s="15"/>
     </row>
-    <row r="9" spans="2:36" ht="18.75">
+    <row r="9" spans="2:36" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B9" s="14"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
@@ -9541,7 +9594,7 @@
       <c r="AI9" s="34"/>
       <c r="AJ9" s="15"/>
     </row>
-    <row r="10" spans="2:36">
+    <row r="10" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B10" s="14"/>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
@@ -9577,7 +9630,7 @@
       <c r="AI10" s="10"/>
       <c r="AJ10" s="15"/>
     </row>
-    <row r="11" spans="2:36">
+    <row r="11" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B11" s="14"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
@@ -9613,7 +9666,7 @@
       <c r="AI11" s="10"/>
       <c r="AJ11" s="15"/>
     </row>
-    <row r="12" spans="2:36">
+    <row r="12" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B12" s="14"/>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
@@ -9649,7 +9702,7 @@
       <c r="AI12" s="10"/>
       <c r="AJ12" s="15"/>
     </row>
-    <row r="13" spans="2:36">
+    <row r="13" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B13" s="14"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
@@ -9684,7 +9737,7 @@
       <c r="AI13" s="10"/>
       <c r="AJ13" s="15"/>
     </row>
-    <row r="14" spans="2:36">
+    <row r="14" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B14" s="14"/>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
@@ -9720,7 +9773,7 @@
       <c r="AI14" s="10"/>
       <c r="AJ14" s="15"/>
     </row>
-    <row r="15" spans="2:36">
+    <row r="15" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B15" s="14"/>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
@@ -9756,7 +9809,7 @@
       <c r="AI15" s="10"/>
       <c r="AJ15" s="15"/>
     </row>
-    <row r="16" spans="2:36">
+    <row r="16" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B16" s="14"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
@@ -9792,7 +9845,7 @@
       <c r="AI16" s="10"/>
       <c r="AJ16" s="15"/>
     </row>
-    <row r="17" spans="2:36">
+    <row r="17" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B17" s="14"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
@@ -9828,7 +9881,7 @@
       <c r="AI17" s="10"/>
       <c r="AJ17" s="15"/>
     </row>
-    <row r="18" spans="2:36">
+    <row r="18" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B18" s="14"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
@@ -9864,7 +9917,7 @@
       <c r="AI18" s="10"/>
       <c r="AJ18" s="15"/>
     </row>
-    <row r="19" spans="2:36">
+    <row r="19" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B19" s="14"/>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
@@ -9900,7 +9953,7 @@
       <c r="AI19" s="10"/>
       <c r="AJ19" s="15"/>
     </row>
-    <row r="20" spans="2:36">
+    <row r="20" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B20" s="14"/>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
@@ -9936,7 +9989,7 @@
       <c r="AI20" s="10"/>
       <c r="AJ20" s="15"/>
     </row>
-    <row r="21" spans="2:36">
+    <row r="21" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B21" s="14"/>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
@@ -9972,7 +10025,7 @@
       <c r="AI21" s="10"/>
       <c r="AJ21" s="15"/>
     </row>
-    <row r="22" spans="2:36">
+    <row r="22" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B22" s="14"/>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
@@ -10008,7 +10061,7 @@
       <c r="AI22" s="10"/>
       <c r="AJ22" s="15"/>
     </row>
-    <row r="23" spans="2:36">
+    <row r="23" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B23" s="14"/>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
@@ -10044,7 +10097,7 @@
       <c r="AI23" s="10"/>
       <c r="AJ23" s="15"/>
     </row>
-    <row r="24" spans="2:36">
+    <row r="24" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B24" s="14"/>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
@@ -10080,7 +10133,7 @@
       <c r="AI24" s="10"/>
       <c r="AJ24" s="15"/>
     </row>
-    <row r="25" spans="2:36">
+    <row r="25" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B25" s="14"/>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
@@ -10116,7 +10169,7 @@
       <c r="AI25" s="10"/>
       <c r="AJ25" s="15"/>
     </row>
-    <row r="26" spans="2:36">
+    <row r="26" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B26" s="14"/>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
@@ -10152,7 +10205,7 @@
       <c r="AI26" s="10"/>
       <c r="AJ26" s="15"/>
     </row>
-    <row r="27" spans="2:36">
+    <row r="27" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B27" s="14"/>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
@@ -10188,7 +10241,7 @@
       <c r="AI27" s="10"/>
       <c r="AJ27" s="15"/>
     </row>
-    <row r="28" spans="2:36">
+    <row r="28" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B28" s="14"/>
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
@@ -10223,7 +10276,7 @@
       <c r="AI28" s="10"/>
       <c r="AJ28" s="15"/>
     </row>
-    <row r="29" spans="2:36">
+    <row r="29" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B29" s="14"/>
       <c r="C29" s="10"/>
       <c r="D29" s="10"/>
@@ -10258,7 +10311,7 @@
       <c r="AI29" s="10"/>
       <c r="AJ29" s="15"/>
     </row>
-    <row r="30" spans="2:36">
+    <row r="30" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B30" s="14"/>
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
@@ -10294,7 +10347,7 @@
       <c r="AI30" s="10"/>
       <c r="AJ30" s="15"/>
     </row>
-    <row r="31" spans="2:36">
+    <row r="31" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B31" s="14"/>
       <c r="C31" s="10"/>
       <c r="D31" s="10"/>
@@ -10330,7 +10383,7 @@
       <c r="AI31" s="10"/>
       <c r="AJ31" s="15"/>
     </row>
-    <row r="32" spans="2:36">
+    <row r="32" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B32" s="14"/>
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
@@ -10366,7 +10419,7 @@
       <c r="AI32" s="10"/>
       <c r="AJ32" s="15"/>
     </row>
-    <row r="33" spans="2:36">
+    <row r="33" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B33" s="14"/>
       <c r="C33" s="10"/>
       <c r="D33" s="10"/>
@@ -10402,7 +10455,7 @@
       <c r="AI33" s="10"/>
       <c r="AJ33" s="15"/>
     </row>
-    <row r="34" spans="2:36">
+    <row r="34" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B34" s="14"/>
       <c r="C34" s="10"/>
       <c r="D34" s="10"/>
@@ -10438,7 +10491,7 @@
       <c r="AI34" s="10"/>
       <c r="AJ34" s="15"/>
     </row>
-    <row r="35" spans="2:36">
+    <row r="35" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B35" s="14"/>
       <c r="C35" s="10"/>
       <c r="D35" s="10"/>
@@ -10474,7 +10527,7 @@
       <c r="AI35" s="10"/>
       <c r="AJ35" s="15"/>
     </row>
-    <row r="36" spans="2:36">
+    <row r="36" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B36" s="14"/>
       <c r="C36" s="10"/>
       <c r="D36" s="10"/>
@@ -10510,7 +10563,7 @@
       <c r="AI36" s="10"/>
       <c r="AJ36" s="15"/>
     </row>
-    <row r="37" spans="2:36">
+    <row r="37" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B37" s="14"/>
       <c r="C37" s="10"/>
       <c r="D37" s="10"/>
@@ -10546,7 +10599,7 @@
       <c r="AI37" s="10"/>
       <c r="AJ37" s="15"/>
     </row>
-    <row r="38" spans="2:36">
+    <row r="38" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B38" s="14"/>
       <c r="C38" s="10"/>
       <c r="D38" s="10"/>
@@ -10582,7 +10635,7 @@
       <c r="AI38" s="10"/>
       <c r="AJ38" s="15"/>
     </row>
-    <row r="39" spans="2:36">
+    <row r="39" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B39" s="14"/>
       <c r="C39" s="10"/>
       <c r="D39" s="10"/>
@@ -10618,7 +10671,7 @@
       <c r="AI39" s="10"/>
       <c r="AJ39" s="15"/>
     </row>
-    <row r="40" spans="2:36">
+    <row r="40" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B40" s="16"/>
       <c r="C40" s="17"/>
       <c r="D40" s="17"/>
@@ -10654,7 +10707,7 @@
       <c r="AI40" s="17"/>
       <c r="AJ40" s="18"/>
     </row>
-    <row r="43" spans="2:36">
+    <row r="43" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B43" s="2"/>
       <c r="C43" s="30" t="s">
         <v>21</v>
@@ -10675,7 +10728,7 @@
       <c r="Q43" s="3"/>
       <c r="R43" s="4"/>
     </row>
-    <row r="44" spans="2:36">
+    <row r="44" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B44" s="5"/>
       <c r="C44" s="19"/>
       <c r="D44" s="1"/>
@@ -10694,7 +10747,7 @@
       <c r="Q44" s="1"/>
       <c r="R44" s="6"/>
     </row>
-    <row r="45" spans="2:36">
+    <row r="45" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B45" s="5"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
@@ -10713,7 +10766,7 @@
       <c r="Q45" s="1"/>
       <c r="R45" s="6"/>
     </row>
-    <row r="46" spans="2:36">
+    <row r="46" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B46" s="5"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -10728,13 +10781,13 @@
       <c r="M46" s="1"/>
       <c r="N46" s="1"/>
       <c r="O46" s="1"/>
-      <c r="P46" s="37" t="s">
+      <c r="P46" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="Q46" s="37"/>
+      <c r="Q46" s="38"/>
       <c r="R46" s="6"/>
     </row>
-    <row r="47" spans="2:36" ht="15" customHeight="1">
+    <row r="47" spans="2:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="5"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
@@ -10755,7 +10808,7 @@
       <c r="Q47" s="32"/>
       <c r="R47" s="6"/>
     </row>
-    <row r="48" spans="2:36" ht="15" customHeight="1">
+    <row r="48" spans="2:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="5"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
@@ -10774,7 +10827,7 @@
       <c r="Q48" s="32"/>
       <c r="R48" s="6"/>
     </row>
-    <row r="49" spans="2:18" ht="18.75">
+    <row r="49" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B49" s="5"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
@@ -10795,7 +10848,7 @@
       <c r="Q49" s="33"/>
       <c r="R49" s="6"/>
     </row>
-    <row r="50" spans="2:18">
+    <row r="50" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B50" s="5"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
@@ -10814,7 +10867,7 @@
       <c r="Q50" s="1"/>
       <c r="R50" s="6"/>
     </row>
-    <row r="51" spans="2:18">
+    <row r="51" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B51" s="5"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
@@ -10833,7 +10886,7 @@
       <c r="Q51" s="1"/>
       <c r="R51" s="6"/>
     </row>
-    <row r="52" spans="2:18">
+    <row r="52" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B52" s="5"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
@@ -10852,7 +10905,7 @@
       <c r="Q52" s="1"/>
       <c r="R52" s="6"/>
     </row>
-    <row r="53" spans="2:18">
+    <row r="53" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B53" s="5"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
@@ -10871,7 +10924,7 @@
       <c r="Q53" s="1"/>
       <c r="R53" s="6"/>
     </row>
-    <row r="54" spans="2:18">
+    <row r="54" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B54" s="5"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
@@ -10890,7 +10943,7 @@
       <c r="Q54" s="1"/>
       <c r="R54" s="6"/>
     </row>
-    <row r="55" spans="2:18">
+    <row r="55" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B55" s="5"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
@@ -10909,7 +10962,7 @@
       <c r="Q55" s="1"/>
       <c r="R55" s="6"/>
     </row>
-    <row r="56" spans="2:18">
+    <row r="56" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B56" s="5"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
@@ -10928,7 +10981,7 @@
       <c r="Q56" s="1"/>
       <c r="R56" s="6"/>
     </row>
-    <row r="57" spans="2:18">
+    <row r="57" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B57" s="5"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
@@ -10947,7 +11000,7 @@
       <c r="Q57" s="1"/>
       <c r="R57" s="6"/>
     </row>
-    <row r="58" spans="2:18">
+    <row r="58" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B58" s="5"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
@@ -10966,7 +11019,7 @@
       <c r="Q58" s="1"/>
       <c r="R58" s="6"/>
     </row>
-    <row r="59" spans="2:18">
+    <row r="59" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B59" s="5"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
@@ -10985,7 +11038,7 @@
       <c r="Q59" s="1"/>
       <c r="R59" s="6"/>
     </row>
-    <row r="60" spans="2:18">
+    <row r="60" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B60" s="5"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
@@ -11004,7 +11057,7 @@
       <c r="Q60" s="1"/>
       <c r="R60" s="6"/>
     </row>
-    <row r="61" spans="2:18">
+    <row r="61" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B61" s="5"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
@@ -11023,7 +11076,7 @@
       <c r="Q61" s="1"/>
       <c r="R61" s="6"/>
     </row>
-    <row r="62" spans="2:18">
+    <row r="62" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B62" s="5"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
@@ -11042,7 +11095,7 @@
       <c r="Q62" s="1"/>
       <c r="R62" s="6"/>
     </row>
-    <row r="63" spans="2:18">
+    <row r="63" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B63" s="5"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
@@ -11061,7 +11114,7 @@
       <c r="Q63" s="1"/>
       <c r="R63" s="6"/>
     </row>
-    <row r="64" spans="2:18">
+    <row r="64" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B64" s="5"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
@@ -11080,7 +11133,7 @@
       <c r="Q64" s="1"/>
       <c r="R64" s="6"/>
     </row>
-    <row r="65" spans="2:18">
+    <row r="65" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B65" s="5"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
@@ -11099,7 +11152,7 @@
       <c r="Q65" s="1"/>
       <c r="R65" s="6"/>
     </row>
-    <row r="66" spans="2:18">
+    <row r="66" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B66" s="5"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
@@ -11118,7 +11171,7 @@
       <c r="Q66" s="1"/>
       <c r="R66" s="6"/>
     </row>
-    <row r="67" spans="2:18">
+    <row r="67" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B67" s="5"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
@@ -11137,7 +11190,7 @@
       <c r="Q67" s="1"/>
       <c r="R67" s="6"/>
     </row>
-    <row r="68" spans="2:18">
+    <row r="68" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B68" s="5"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
@@ -11156,7 +11209,7 @@
       <c r="Q68" s="1"/>
       <c r="R68" s="6"/>
     </row>
-    <row r="69" spans="2:18">
+    <row r="69" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B69" s="5"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
@@ -11175,7 +11228,7 @@
       <c r="Q69" s="1"/>
       <c r="R69" s="6"/>
     </row>
-    <row r="70" spans="2:18">
+    <row r="70" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B70" s="5"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
@@ -11194,7 +11247,7 @@
       <c r="Q70" s="1"/>
       <c r="R70" s="6"/>
     </row>
-    <row r="71" spans="2:18">
+    <row r="71" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B71" s="5"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
@@ -11213,7 +11266,7 @@
       <c r="Q71" s="1"/>
       <c r="R71" s="6"/>
     </row>
-    <row r="72" spans="2:18">
+    <row r="72" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B72" s="5"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
@@ -11232,7 +11285,7 @@
       <c r="Q72" s="1"/>
       <c r="R72" s="6"/>
     </row>
-    <row r="73" spans="2:18">
+    <row r="73" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B73" s="5"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
@@ -11251,7 +11304,7 @@
       <c r="Q73" s="1"/>
       <c r="R73" s="6"/>
     </row>
-    <row r="74" spans="2:18">
+    <row r="74" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B74" s="5"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
@@ -11270,7 +11323,7 @@
       <c r="Q74" s="1"/>
       <c r="R74" s="6"/>
     </row>
-    <row r="75" spans="2:18">
+    <row r="75" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B75" s="5"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
@@ -11289,7 +11342,7 @@
       <c r="Q75" s="1"/>
       <c r="R75" s="6"/>
     </row>
-    <row r="76" spans="2:18">
+    <row r="76" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B76" s="5"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
@@ -11308,7 +11361,7 @@
       <c r="Q76" s="1"/>
       <c r="R76" s="6"/>
     </row>
-    <row r="77" spans="2:18">
+    <row r="77" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B77" s="5"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
@@ -11327,7 +11380,7 @@
       <c r="Q77" s="1"/>
       <c r="R77" s="6"/>
     </row>
-    <row r="78" spans="2:18">
+    <row r="78" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B78" s="5"/>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
@@ -11346,7 +11399,7 @@
       <c r="Q78" s="1"/>
       <c r="R78" s="6"/>
     </row>
-    <row r="79" spans="2:18">
+    <row r="79" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B79" s="5"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
@@ -11365,7 +11418,7 @@
       <c r="Q79" s="1"/>
       <c r="R79" s="6"/>
     </row>
-    <row r="80" spans="2:18">
+    <row r="80" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B80" s="7"/>
       <c r="C80" s="8"/>
       <c r="D80" s="8"/>
@@ -11384,63 +11437,63 @@
       <c r="Q80" s="8"/>
       <c r="R80" s="9"/>
     </row>
-    <row r="85" spans="2:18">
-      <c r="B85" s="38" t="s">
+    <row r="85" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B85" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="C85" s="38"/>
-      <c r="D85" s="38"/>
-      <c r="E85" s="38"/>
-      <c r="F85" s="38"/>
-      <c r="G85" s="38"/>
-      <c r="H85" s="38"/>
-      <c r="I85" s="38"/>
-      <c r="J85" s="38"/>
-      <c r="K85" s="38"/>
-      <c r="L85" s="38"/>
-      <c r="M85" s="38"/>
-      <c r="N85" s="38"/>
-      <c r="O85" s="38"/>
-      <c r="P85" s="38"/>
-      <c r="Q85" s="38"/>
-      <c r="R85" s="38"/>
-    </row>
-    <row r="86" spans="2:18">
-      <c r="B86" s="38"/>
-      <c r="C86" s="38"/>
-      <c r="D86" s="38"/>
-      <c r="E86" s="38"/>
-      <c r="F86" s="38"/>
-      <c r="G86" s="38"/>
-      <c r="H86" s="38"/>
-      <c r="I86" s="38"/>
-      <c r="J86" s="38"/>
-      <c r="K86" s="38"/>
-      <c r="L86" s="38"/>
-      <c r="M86" s="38"/>
-      <c r="N86" s="38"/>
-      <c r="O86" s="38"/>
-      <c r="P86" s="38"/>
-      <c r="Q86" s="38"/>
-      <c r="R86" s="38"/>
-    </row>
-    <row r="89" spans="2:18">
+      <c r="C85" s="37"/>
+      <c r="D85" s="37"/>
+      <c r="E85" s="37"/>
+      <c r="F85" s="37"/>
+      <c r="G85" s="37"/>
+      <c r="H85" s="37"/>
+      <c r="I85" s="37"/>
+      <c r="J85" s="37"/>
+      <c r="K85" s="37"/>
+      <c r="L85" s="37"/>
+      <c r="M85" s="37"/>
+      <c r="N85" s="37"/>
+      <c r="O85" s="37"/>
+      <c r="P85" s="37"/>
+      <c r="Q85" s="37"/>
+      <c r="R85" s="37"/>
+    </row>
+    <row r="86" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B86" s="37"/>
+      <c r="C86" s="37"/>
+      <c r="D86" s="37"/>
+      <c r="E86" s="37"/>
+      <c r="F86" s="37"/>
+      <c r="G86" s="37"/>
+      <c r="H86" s="37"/>
+      <c r="I86" s="37"/>
+      <c r="J86" s="37"/>
+      <c r="K86" s="37"/>
+      <c r="L86" s="37"/>
+      <c r="M86" s="37"/>
+      <c r="N86" s="37"/>
+      <c r="O86" s="37"/>
+      <c r="P86" s="37"/>
+      <c r="Q86" s="37"/>
+      <c r="R86" s="37"/>
+    </row>
+    <row r="89" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E89" s="23" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="AH6:AI6"/>
+    <mergeCell ref="P7:Q8"/>
+    <mergeCell ref="AH7:AI8"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="AH9:AI9"/>
     <mergeCell ref="B85:R86"/>
     <mergeCell ref="P46:Q46"/>
     <mergeCell ref="P47:Q48"/>
     <mergeCell ref="P49:Q49"/>
     <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="AH6:AI6"/>
-    <mergeCell ref="P7:Q8"/>
-    <mergeCell ref="AH7:AI8"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="AH9:AI9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -11452,13 +11505,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF690D20-3AF0-4911-A815-03050030AE1D}">
   <dimension ref="B2:AJ79"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AH59" sqref="AH59"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A18" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AR27" sqref="AR27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:36">
+    <row r="2" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B2" s="11"/>
       <c r="C2" s="30" t="s">
         <v>22</v>
@@ -11498,7 +11551,7 @@
       <c r="AI2" s="12"/>
       <c r="AJ2" s="13"/>
     </row>
-    <row r="3" spans="2:36">
+    <row r="3" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B3" s="14"/>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
@@ -11534,7 +11587,7 @@
       <c r="AI3" s="10"/>
       <c r="AJ3" s="15"/>
     </row>
-    <row r="4" spans="2:36">
+    <row r="4" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B4" s="14"/>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -11570,7 +11623,7 @@
       <c r="AI4" s="10"/>
       <c r="AJ4" s="15"/>
     </row>
-    <row r="5" spans="2:36">
+    <row r="5" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B5" s="14"/>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
@@ -11585,10 +11638,10 @@
       <c r="M5" s="10"/>
       <c r="N5" s="10"/>
       <c r="O5" s="10"/>
-      <c r="P5" s="37" t="s">
+      <c r="P5" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="Q5" s="37"/>
+      <c r="Q5" s="38"/>
       <c r="R5" s="15"/>
       <c r="T5" s="14"/>
       <c r="U5" s="10"/>
@@ -11604,13 +11657,13 @@
       <c r="AE5" s="10"/>
       <c r="AF5" s="10"/>
       <c r="AG5" s="10"/>
-      <c r="AH5" s="37" t="s">
+      <c r="AH5" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="AI5" s="37"/>
+      <c r="AI5" s="38"/>
       <c r="AJ5" s="15"/>
     </row>
-    <row r="6" spans="2:36">
+    <row r="6" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B6" s="14"/>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
@@ -11650,7 +11703,7 @@
       <c r="AI6" s="36"/>
       <c r="AJ6" s="15"/>
     </row>
-    <row r="7" spans="2:36">
+    <row r="7" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B7" s="14"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -11686,7 +11739,7 @@
       <c r="AI7" s="36"/>
       <c r="AJ7" s="15"/>
     </row>
-    <row r="8" spans="2:36" ht="18.75">
+    <row r="8" spans="2:36" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B8" s="14"/>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
@@ -11726,7 +11779,7 @@
       <c r="AI8" s="34"/>
       <c r="AJ8" s="15"/>
     </row>
-    <row r="9" spans="2:36">
+    <row r="9" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B9" s="14"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
@@ -11762,7 +11815,7 @@
       <c r="AI9" s="10"/>
       <c r="AJ9" s="15"/>
     </row>
-    <row r="10" spans="2:36">
+    <row r="10" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B10" s="14"/>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
@@ -11797,7 +11850,7 @@
       <c r="AI10" s="10"/>
       <c r="AJ10" s="15"/>
     </row>
-    <row r="11" spans="2:36">
+    <row r="11" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B11" s="14"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
@@ -11833,7 +11886,7 @@
       <c r="AI11" s="10"/>
       <c r="AJ11" s="15"/>
     </row>
-    <row r="12" spans="2:36">
+    <row r="12" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B12" s="14"/>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
@@ -11869,7 +11922,7 @@
       <c r="AI12" s="10"/>
       <c r="AJ12" s="15"/>
     </row>
-    <row r="13" spans="2:36">
+    <row r="13" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B13" s="14"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
@@ -11904,7 +11957,7 @@
       <c r="AI13" s="10"/>
       <c r="AJ13" s="15"/>
     </row>
-    <row r="14" spans="2:36">
+    <row r="14" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B14" s="14"/>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
@@ -11940,7 +11993,7 @@
       <c r="AI14" s="10"/>
       <c r="AJ14" s="15"/>
     </row>
-    <row r="15" spans="2:36">
+    <row r="15" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B15" s="14"/>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
@@ -11976,7 +12029,7 @@
       <c r="AI15" s="10"/>
       <c r="AJ15" s="15"/>
     </row>
-    <row r="16" spans="2:36">
+    <row r="16" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B16" s="14"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
@@ -12012,7 +12065,7 @@
       <c r="AI16" s="10"/>
       <c r="AJ16" s="15"/>
     </row>
-    <row r="17" spans="2:36">
+    <row r="17" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B17" s="14"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
@@ -12048,7 +12101,7 @@
       <c r="AI17" s="10"/>
       <c r="AJ17" s="15"/>
     </row>
-    <row r="18" spans="2:36">
+    <row r="18" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B18" s="14"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
@@ -12084,7 +12137,7 @@
       <c r="AI18" s="10"/>
       <c r="AJ18" s="15"/>
     </row>
-    <row r="19" spans="2:36">
+    <row r="19" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B19" s="14"/>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
@@ -12120,7 +12173,7 @@
       <c r="AI19" s="10"/>
       <c r="AJ19" s="15"/>
     </row>
-    <row r="20" spans="2:36">
+    <row r="20" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B20" s="14"/>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
@@ -12156,7 +12209,7 @@
       <c r="AI20" s="10"/>
       <c r="AJ20" s="15"/>
     </row>
-    <row r="21" spans="2:36">
+    <row r="21" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B21" s="14"/>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
@@ -12192,7 +12245,7 @@
       <c r="AI21" s="10"/>
       <c r="AJ21" s="15"/>
     </row>
-    <row r="22" spans="2:36">
+    <row r="22" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B22" s="14"/>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
@@ -12227,7 +12280,7 @@
       <c r="AI22" s="10"/>
       <c r="AJ22" s="15"/>
     </row>
-    <row r="23" spans="2:36">
+    <row r="23" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B23" s="14"/>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
@@ -12262,7 +12315,7 @@
       <c r="AI23" s="10"/>
       <c r="AJ23" s="15"/>
     </row>
-    <row r="24" spans="2:36">
+    <row r="24" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B24" s="14"/>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
@@ -12298,7 +12351,7 @@
       <c r="AI24" s="10"/>
       <c r="AJ24" s="15"/>
     </row>
-    <row r="25" spans="2:36">
+    <row r="25" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B25" s="14"/>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
@@ -12334,7 +12387,7 @@
       <c r="AI25" s="10"/>
       <c r="AJ25" s="15"/>
     </row>
-    <row r="26" spans="2:36">
+    <row r="26" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B26" s="14"/>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
@@ -12370,7 +12423,7 @@
       <c r="AI26" s="10"/>
       <c r="AJ26" s="15"/>
     </row>
-    <row r="27" spans="2:36">
+    <row r="27" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B27" s="14"/>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
@@ -12406,7 +12459,7 @@
       <c r="AI27" s="10"/>
       <c r="AJ27" s="15"/>
     </row>
-    <row r="28" spans="2:36">
+    <row r="28" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B28" s="14"/>
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
@@ -12442,7 +12495,7 @@
       <c r="AI28" s="10"/>
       <c r="AJ28" s="15"/>
     </row>
-    <row r="29" spans="2:36">
+    <row r="29" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B29" s="14"/>
       <c r="C29" s="10"/>
       <c r="D29" s="10"/>
@@ -12478,7 +12531,7 @@
       <c r="AI29" s="10"/>
       <c r="AJ29" s="15"/>
     </row>
-    <row r="30" spans="2:36">
+    <row r="30" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B30" s="14"/>
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
@@ -12514,7 +12567,7 @@
       <c r="AI30" s="10"/>
       <c r="AJ30" s="15"/>
     </row>
-    <row r="31" spans="2:36">
+    <row r="31" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B31" s="14"/>
       <c r="C31" s="10"/>
       <c r="D31" s="10"/>
@@ -12550,7 +12603,7 @@
       <c r="AI31" s="10"/>
       <c r="AJ31" s="15"/>
     </row>
-    <row r="32" spans="2:36">
+    <row r="32" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B32" s="14"/>
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
@@ -12586,7 +12639,7 @@
       <c r="AI32" s="10"/>
       <c r="AJ32" s="15"/>
     </row>
-    <row r="33" spans="2:36">
+    <row r="33" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B33" s="14"/>
       <c r="C33" s="10"/>
       <c r="D33" s="10"/>
@@ -12622,7 +12675,7 @@
       <c r="AI33" s="10"/>
       <c r="AJ33" s="15"/>
     </row>
-    <row r="34" spans="2:36">
+    <row r="34" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B34" s="14"/>
       <c r="C34" s="10"/>
       <c r="D34" s="10"/>
@@ -12658,7 +12711,7 @@
       <c r="AI34" s="10"/>
       <c r="AJ34" s="15"/>
     </row>
-    <row r="35" spans="2:36">
+    <row r="35" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B35" s="14"/>
       <c r="C35" s="10"/>
       <c r="D35" s="10"/>
@@ -12694,7 +12747,7 @@
       <c r="AI35" s="10"/>
       <c r="AJ35" s="15"/>
     </row>
-    <row r="36" spans="2:36">
+    <row r="36" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B36" s="14"/>
       <c r="C36" s="10"/>
       <c r="D36" s="10"/>
@@ -12730,7 +12783,7 @@
       <c r="AI36" s="10"/>
       <c r="AJ36" s="15"/>
     </row>
-    <row r="37" spans="2:36">
+    <row r="37" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B37" s="14"/>
       <c r="C37" s="10"/>
       <c r="D37" s="10"/>
@@ -12766,7 +12819,7 @@
       <c r="AI37" s="10"/>
       <c r="AJ37" s="15"/>
     </row>
-    <row r="38" spans="2:36">
+    <row r="38" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B38" s="14"/>
       <c r="C38" s="10"/>
       <c r="D38" s="10"/>
@@ -12802,7 +12855,7 @@
       <c r="AI38" s="10"/>
       <c r="AJ38" s="15"/>
     </row>
-    <row r="39" spans="2:36">
+    <row r="39" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B39" s="16"/>
       <c r="C39" s="17"/>
       <c r="D39" s="17"/>
@@ -12838,7 +12891,7 @@
       <c r="AI39" s="17"/>
       <c r="AJ39" s="18"/>
     </row>
-    <row r="42" spans="2:36">
+    <row r="42" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B42" s="2"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
@@ -12857,7 +12910,7 @@
       <c r="Q42" s="3"/>
       <c r="R42" s="4"/>
     </row>
-    <row r="43" spans="2:36">
+    <row r="43" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B43" s="5"/>
       <c r="C43" s="19"/>
       <c r="D43" s="23" t="s">
@@ -12878,7 +12931,7 @@
       <c r="Q43" s="1"/>
       <c r="R43" s="6"/>
     </row>
-    <row r="44" spans="2:36">
+    <row r="44" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B44" s="5"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -12897,7 +12950,7 @@
       <c r="Q44" s="1"/>
       <c r="R44" s="6"/>
     </row>
-    <row r="45" spans="2:36">
+    <row r="45" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B45" s="5"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
@@ -12912,13 +12965,13 @@
       <c r="M45" s="1"/>
       <c r="N45" s="1"/>
       <c r="O45" s="1"/>
-      <c r="P45" s="37" t="s">
+      <c r="P45" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="Q45" s="37"/>
+      <c r="Q45" s="38"/>
       <c r="R45" s="6"/>
     </row>
-    <row r="46" spans="2:36">
+    <row r="46" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B46" s="5"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -12939,7 +12992,7 @@
       <c r="Q46" s="32"/>
       <c r="R46" s="6"/>
     </row>
-    <row r="47" spans="2:36">
+    <row r="47" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B47" s="5"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
@@ -12958,7 +13011,7 @@
       <c r="Q47" s="32"/>
       <c r="R47" s="6"/>
     </row>
-    <row r="48" spans="2:36" ht="18.75">
+    <row r="48" spans="2:36" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B48" s="5"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
@@ -12979,7 +13032,7 @@
       <c r="Q48" s="33"/>
       <c r="R48" s="6"/>
     </row>
-    <row r="49" spans="2:18">
+    <row r="49" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B49" s="5"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
@@ -12998,7 +13051,7 @@
       <c r="Q49" s="1"/>
       <c r="R49" s="6"/>
     </row>
-    <row r="50" spans="2:18">
+    <row r="50" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B50" s="5"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
@@ -13017,7 +13070,7 @@
       <c r="Q50" s="1"/>
       <c r="R50" s="6"/>
     </row>
-    <row r="51" spans="2:18">
+    <row r="51" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B51" s="5"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
@@ -13036,7 +13089,7 @@
       <c r="Q51" s="1"/>
       <c r="R51" s="6"/>
     </row>
-    <row r="52" spans="2:18">
+    <row r="52" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B52" s="5"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
@@ -13055,7 +13108,7 @@
       <c r="Q52" s="1"/>
       <c r="R52" s="6"/>
     </row>
-    <row r="53" spans="2:18">
+    <row r="53" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B53" s="5"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
@@ -13074,7 +13127,7 @@
       <c r="Q53" s="1"/>
       <c r="R53" s="6"/>
     </row>
-    <row r="54" spans="2:18">
+    <row r="54" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B54" s="5"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
@@ -13093,7 +13146,7 @@
       <c r="Q54" s="1"/>
       <c r="R54" s="6"/>
     </row>
-    <row r="55" spans="2:18">
+    <row r="55" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B55" s="5"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
@@ -13112,7 +13165,7 @@
       <c r="Q55" s="1"/>
       <c r="R55" s="6"/>
     </row>
-    <row r="56" spans="2:18">
+    <row r="56" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B56" s="5"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
@@ -13131,7 +13184,7 @@
       <c r="Q56" s="1"/>
       <c r="R56" s="6"/>
     </row>
-    <row r="57" spans="2:18">
+    <row r="57" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B57" s="5"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
@@ -13150,7 +13203,7 @@
       <c r="Q57" s="1"/>
       <c r="R57" s="6"/>
     </row>
-    <row r="58" spans="2:18">
+    <row r="58" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B58" s="5"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
@@ -13169,7 +13222,7 @@
       <c r="Q58" s="1"/>
       <c r="R58" s="6"/>
     </row>
-    <row r="59" spans="2:18">
+    <row r="59" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B59" s="5"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
@@ -13188,7 +13241,7 @@
       <c r="Q59" s="1"/>
       <c r="R59" s="6"/>
     </row>
-    <row r="60" spans="2:18">
+    <row r="60" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B60" s="5"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
@@ -13207,7 +13260,7 @@
       <c r="Q60" s="1"/>
       <c r="R60" s="6"/>
     </row>
-    <row r="61" spans="2:18">
+    <row r="61" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B61" s="5"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
@@ -13225,7 +13278,7 @@
       <c r="Q61" s="1"/>
       <c r="R61" s="6"/>
     </row>
-    <row r="62" spans="2:18">
+    <row r="62" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B62" s="5"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
@@ -13244,7 +13297,7 @@
       <c r="Q62" s="1"/>
       <c r="R62" s="6"/>
     </row>
-    <row r="63" spans="2:18">
+    <row r="63" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B63" s="5"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
@@ -13263,7 +13316,7 @@
       <c r="Q63" s="1"/>
       <c r="R63" s="6"/>
     </row>
-    <row r="64" spans="2:18">
+    <row r="64" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B64" s="5"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
@@ -13282,7 +13335,7 @@
       <c r="Q64" s="1"/>
       <c r="R64" s="6"/>
     </row>
-    <row r="65" spans="2:18">
+    <row r="65" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B65" s="5"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
@@ -13301,7 +13354,7 @@
       <c r="Q65" s="1"/>
       <c r="R65" s="6"/>
     </row>
-    <row r="66" spans="2:18">
+    <row r="66" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B66" s="5"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
@@ -13320,7 +13373,7 @@
       <c r="Q66" s="1"/>
       <c r="R66" s="6"/>
     </row>
-    <row r="67" spans="2:18">
+    <row r="67" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B67" s="5"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
@@ -13339,7 +13392,7 @@
       <c r="Q67" s="1"/>
       <c r="R67" s="6"/>
     </row>
-    <row r="68" spans="2:18">
+    <row r="68" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B68" s="5"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
@@ -13358,7 +13411,7 @@
       <c r="Q68" s="1"/>
       <c r="R68" s="6"/>
     </row>
-    <row r="69" spans="2:18">
+    <row r="69" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B69" s="5"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
@@ -13377,7 +13430,7 @@
       <c r="Q69" s="1"/>
       <c r="R69" s="6"/>
     </row>
-    <row r="70" spans="2:18">
+    <row r="70" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B70" s="5"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
@@ -13396,7 +13449,7 @@
       <c r="Q70" s="1"/>
       <c r="R70" s="6"/>
     </row>
-    <row r="71" spans="2:18">
+    <row r="71" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B71" s="5"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
@@ -13415,7 +13468,7 @@
       <c r="Q71" s="1"/>
       <c r="R71" s="6"/>
     </row>
-    <row r="72" spans="2:18">
+    <row r="72" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B72" s="5"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
@@ -13434,7 +13487,7 @@
       <c r="Q72" s="1"/>
       <c r="R72" s="6"/>
     </row>
-    <row r="73" spans="2:18">
+    <row r="73" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B73" s="5"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
@@ -13453,7 +13506,7 @@
       <c r="Q73" s="1"/>
       <c r="R73" s="6"/>
     </row>
-    <row r="74" spans="2:18">
+    <row r="74" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B74" s="5"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
@@ -13472,7 +13525,7 @@
       <c r="Q74" s="1"/>
       <c r="R74" s="6"/>
     </row>
-    <row r="75" spans="2:18">
+    <row r="75" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B75" s="5"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
@@ -13491,7 +13544,7 @@
       <c r="Q75" s="1"/>
       <c r="R75" s="6"/>
     </row>
-    <row r="76" spans="2:18">
+    <row r="76" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B76" s="5"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
@@ -13510,7 +13563,7 @@
       <c r="Q76" s="1"/>
       <c r="R76" s="6"/>
     </row>
-    <row r="77" spans="2:18">
+    <row r="77" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B77" s="5"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
@@ -13529,7 +13582,7 @@
       <c r="Q77" s="1"/>
       <c r="R77" s="6"/>
     </row>
-    <row r="78" spans="2:18">
+    <row r="78" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B78" s="5"/>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
@@ -13548,7 +13601,7 @@
       <c r="Q78" s="1"/>
       <c r="R78" s="6"/>
     </row>
-    <row r="79" spans="2:18">
+    <row r="79" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B79" s="7"/>
       <c r="C79" s="8"/>
       <c r="D79" s="8"/>
@@ -13589,13 +13642,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F21EAB9-BF43-48C4-8C18-F2ACFC45CB60}">
   <dimension ref="B2:AJ79"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AJ40" sqref="AJ40"/>
+    <sheetView showGridLines="0" topLeftCell="A33" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AL27" sqref="AL27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:36">
+    <row r="2" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B2" s="11"/>
       <c r="C2" s="12"/>
       <c r="D2" s="23" t="s">
@@ -13633,7 +13686,7 @@
       <c r="AI2" s="12"/>
       <c r="AJ2" s="13"/>
     </row>
-    <row r="3" spans="2:36">
+    <row r="3" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B3" s="14"/>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
@@ -13671,7 +13724,7 @@
       <c r="AI3" s="10"/>
       <c r="AJ3" s="15"/>
     </row>
-    <row r="4" spans="2:36">
+    <row r="4" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B4" s="14"/>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -13707,7 +13760,7 @@
       <c r="AI4" s="10"/>
       <c r="AJ4" s="15"/>
     </row>
-    <row r="5" spans="2:36">
+    <row r="5" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B5" s="14"/>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
@@ -13722,10 +13775,10 @@
       <c r="M5" s="10"/>
       <c r="N5" s="10"/>
       <c r="O5" s="10"/>
-      <c r="P5" s="37" t="s">
+      <c r="P5" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="Q5" s="37"/>
+      <c r="Q5" s="38"/>
       <c r="R5" s="15"/>
       <c r="T5" s="14"/>
       <c r="U5" s="10"/>
@@ -13741,13 +13794,13 @@
       <c r="AE5" s="10"/>
       <c r="AF5" s="10"/>
       <c r="AG5" s="10"/>
-      <c r="AH5" s="37" t="s">
+      <c r="AH5" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="AI5" s="37"/>
+      <c r="AI5" s="38"/>
       <c r="AJ5" s="15"/>
     </row>
-    <row r="6" spans="2:36">
+    <row r="6" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B6" s="14"/>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
@@ -13787,7 +13840,7 @@
       <c r="AI6" s="36"/>
       <c r="AJ6" s="15"/>
     </row>
-    <row r="7" spans="2:36">
+    <row r="7" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B7" s="14"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -13823,7 +13876,7 @@
       <c r="AI7" s="36"/>
       <c r="AJ7" s="15"/>
     </row>
-    <row r="8" spans="2:36" ht="18.75">
+    <row r="8" spans="2:36" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B8" s="14"/>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
@@ -13863,7 +13916,7 @@
       <c r="AI8" s="34"/>
       <c r="AJ8" s="15"/>
     </row>
-    <row r="9" spans="2:36">
+    <row r="9" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B9" s="14"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
@@ -13899,7 +13952,7 @@
       <c r="AI9" s="10"/>
       <c r="AJ9" s="15"/>
     </row>
-    <row r="10" spans="2:36">
+    <row r="10" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B10" s="14"/>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
@@ -13934,7 +13987,7 @@
       <c r="AI10" s="10"/>
       <c r="AJ10" s="15"/>
     </row>
-    <row r="11" spans="2:36">
+    <row r="11" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B11" s="14"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
@@ -13970,7 +14023,7 @@
       <c r="AI11" s="10"/>
       <c r="AJ11" s="15"/>
     </row>
-    <row r="12" spans="2:36">
+    <row r="12" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B12" s="14"/>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
@@ -14006,7 +14059,7 @@
       <c r="AI12" s="10"/>
       <c r="AJ12" s="15"/>
     </row>
-    <row r="13" spans="2:36">
+    <row r="13" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B13" s="14"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
@@ -14042,7 +14095,7 @@
       <c r="AI13" s="10"/>
       <c r="AJ13" s="15"/>
     </row>
-    <row r="14" spans="2:36">
+    <row r="14" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B14" s="14"/>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
@@ -14078,7 +14131,7 @@
       <c r="AI14" s="10"/>
       <c r="AJ14" s="15"/>
     </row>
-    <row r="15" spans="2:36">
+    <row r="15" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B15" s="14"/>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
@@ -14113,7 +14166,7 @@
       <c r="AI15" s="10"/>
       <c r="AJ15" s="15"/>
     </row>
-    <row r="16" spans="2:36">
+    <row r="16" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B16" s="14"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
@@ -14149,7 +14202,7 @@
       <c r="AI16" s="10"/>
       <c r="AJ16" s="15"/>
     </row>
-    <row r="17" spans="2:36">
+    <row r="17" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B17" s="14"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
@@ -14185,7 +14238,7 @@
       <c r="AI17" s="10"/>
       <c r="AJ17" s="15"/>
     </row>
-    <row r="18" spans="2:36">
+    <row r="18" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B18" s="14"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
@@ -14221,7 +14274,7 @@
       <c r="AI18" s="10"/>
       <c r="AJ18" s="15"/>
     </row>
-    <row r="19" spans="2:36">
+    <row r="19" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B19" s="14"/>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
@@ -14257,7 +14310,7 @@
       <c r="AI19" s="10"/>
       <c r="AJ19" s="15"/>
     </row>
-    <row r="20" spans="2:36">
+    <row r="20" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B20" s="14"/>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
@@ -14293,7 +14346,7 @@
       <c r="AI20" s="10"/>
       <c r="AJ20" s="15"/>
     </row>
-    <row r="21" spans="2:36">
+    <row r="21" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B21" s="14"/>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
@@ -14329,7 +14382,7 @@
       <c r="AI21" s="10"/>
       <c r="AJ21" s="15"/>
     </row>
-    <row r="22" spans="2:36">
+    <row r="22" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B22" s="14"/>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
@@ -14365,7 +14418,7 @@
       <c r="AI22" s="10"/>
       <c r="AJ22" s="15"/>
     </row>
-    <row r="23" spans="2:36">
+    <row r="23" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B23" s="14"/>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
@@ -14401,7 +14454,7 @@
       <c r="AI23" s="10"/>
       <c r="AJ23" s="15"/>
     </row>
-    <row r="24" spans="2:36">
+    <row r="24" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B24" s="14"/>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
@@ -14436,7 +14489,7 @@
       <c r="AI24" s="10"/>
       <c r="AJ24" s="15"/>
     </row>
-    <row r="25" spans="2:36">
+    <row r="25" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B25" s="14"/>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
@@ -14472,7 +14525,7 @@
       <c r="AI25" s="10"/>
       <c r="AJ25" s="15"/>
     </row>
-    <row r="26" spans="2:36">
+    <row r="26" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B26" s="14"/>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
@@ -14508,7 +14561,7 @@
       <c r="AI26" s="10"/>
       <c r="AJ26" s="15"/>
     </row>
-    <row r="27" spans="2:36">
+    <row r="27" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B27" s="14"/>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
@@ -14544,7 +14597,7 @@
       <c r="AI27" s="10"/>
       <c r="AJ27" s="15"/>
     </row>
-    <row r="28" spans="2:36">
+    <row r="28" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B28" s="14"/>
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
@@ -14580,7 +14633,7 @@
       <c r="AI28" s="10"/>
       <c r="AJ28" s="15"/>
     </row>
-    <row r="29" spans="2:36">
+    <row r="29" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B29" s="14"/>
       <c r="C29" s="10"/>
       <c r="D29" s="10"/>
@@ -14616,7 +14669,7 @@
       <c r="AI29" s="10"/>
       <c r="AJ29" s="15"/>
     </row>
-    <row r="30" spans="2:36">
+    <row r="30" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B30" s="14"/>
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
@@ -14652,7 +14705,7 @@
       <c r="AI30" s="10"/>
       <c r="AJ30" s="15"/>
     </row>
-    <row r="31" spans="2:36">
+    <row r="31" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B31" s="14"/>
       <c r="C31" s="10"/>
       <c r="D31" s="10"/>
@@ -14688,7 +14741,7 @@
       <c r="AI31" s="10"/>
       <c r="AJ31" s="15"/>
     </row>
-    <row r="32" spans="2:36">
+    <row r="32" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B32" s="14"/>
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
@@ -14724,7 +14777,7 @@
       <c r="AI32" s="10"/>
       <c r="AJ32" s="15"/>
     </row>
-    <row r="33" spans="2:36">
+    <row r="33" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B33" s="14"/>
       <c r="C33" s="10"/>
       <c r="D33" s="10"/>
@@ -14760,7 +14813,7 @@
       <c r="AI33" s="10"/>
       <c r="AJ33" s="15"/>
     </row>
-    <row r="34" spans="2:36">
+    <row r="34" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B34" s="14"/>
       <c r="C34" s="10"/>
       <c r="D34" s="10"/>
@@ -14796,7 +14849,7 @@
       <c r="AI34" s="10"/>
       <c r="AJ34" s="15"/>
     </row>
-    <row r="35" spans="2:36">
+    <row r="35" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B35" s="14"/>
       <c r="C35" s="10"/>
       <c r="D35" s="10"/>
@@ -14832,7 +14885,7 @@
       <c r="AI35" s="10"/>
       <c r="AJ35" s="15"/>
     </row>
-    <row r="36" spans="2:36">
+    <row r="36" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B36" s="14"/>
       <c r="C36" s="10"/>
       <c r="D36" s="10"/>
@@ -14867,7 +14920,7 @@
       <c r="AI36" s="10"/>
       <c r="AJ36" s="15"/>
     </row>
-    <row r="37" spans="2:36">
+    <row r="37" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B37" s="14"/>
       <c r="C37" s="10"/>
       <c r="D37" s="10"/>
@@ -14903,7 +14956,7 @@
       <c r="AI37" s="10"/>
       <c r="AJ37" s="15"/>
     </row>
-    <row r="38" spans="2:36">
+    <row r="38" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B38" s="14"/>
       <c r="C38" s="10"/>
       <c r="D38" s="10"/>
@@ -14939,7 +14992,7 @@
       <c r="AI38" s="10"/>
       <c r="AJ38" s="15"/>
     </row>
-    <row r="39" spans="2:36">
+    <row r="39" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B39" s="16"/>
       <c r="C39" s="17"/>
       <c r="D39" s="17"/>
@@ -14975,7 +15028,7 @@
       <c r="AI39" s="17"/>
       <c r="AJ39" s="18"/>
     </row>
-    <row r="42" spans="2:36">
+    <row r="42" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B42" s="2"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
@@ -14994,7 +15047,7 @@
       <c r="Q42" s="3"/>
       <c r="R42" s="4"/>
     </row>
-    <row r="43" spans="2:36">
+    <row r="43" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B43" s="5"/>
       <c r="C43" s="19"/>
       <c r="D43" s="23" t="s">
@@ -15015,7 +15068,7 @@
       <c r="Q43" s="1"/>
       <c r="R43" s="6"/>
     </row>
-    <row r="44" spans="2:36">
+    <row r="44" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B44" s="5"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -15034,7 +15087,7 @@
       <c r="Q44" s="1"/>
       <c r="R44" s="6"/>
     </row>
-    <row r="45" spans="2:36">
+    <row r="45" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B45" s="5"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
@@ -15049,13 +15102,13 @@
       <c r="M45" s="1"/>
       <c r="N45" s="1"/>
       <c r="O45" s="1"/>
-      <c r="P45" s="37" t="s">
+      <c r="P45" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="Q45" s="37"/>
+      <c r="Q45" s="38"/>
       <c r="R45" s="6"/>
     </row>
-    <row r="46" spans="2:36">
+    <row r="46" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B46" s="5"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
@@ -15075,7 +15128,7 @@
       <c r="Q46" s="32"/>
       <c r="R46" s="6"/>
     </row>
-    <row r="47" spans="2:36">
+    <row r="47" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B47" s="5"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
@@ -15094,7 +15147,7 @@
       <c r="Q47" s="32"/>
       <c r="R47" s="6"/>
     </row>
-    <row r="48" spans="2:36" ht="18.75">
+    <row r="48" spans="2:36" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B48" s="5"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
@@ -15115,7 +15168,7 @@
       <c r="Q48" s="33"/>
       <c r="R48" s="6"/>
     </row>
-    <row r="49" spans="2:18">
+    <row r="49" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B49" s="5"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
@@ -15134,7 +15187,7 @@
       <c r="Q49" s="1"/>
       <c r="R49" s="6"/>
     </row>
-    <row r="50" spans="2:18">
+    <row r="50" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B50" s="5"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
@@ -15153,7 +15206,7 @@
       <c r="Q50" s="1"/>
       <c r="R50" s="6"/>
     </row>
-    <row r="51" spans="2:18">
+    <row r="51" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B51" s="5"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
@@ -15172,7 +15225,7 @@
       <c r="Q51" s="1"/>
       <c r="R51" s="6"/>
     </row>
-    <row r="52" spans="2:18">
+    <row r="52" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B52" s="5"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
@@ -15191,7 +15244,7 @@
       <c r="Q52" s="1"/>
       <c r="R52" s="6"/>
     </row>
-    <row r="53" spans="2:18">
+    <row r="53" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B53" s="5"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
@@ -15210,7 +15263,7 @@
       <c r="Q53" s="1"/>
       <c r="R53" s="6"/>
     </row>
-    <row r="54" spans="2:18">
+    <row r="54" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B54" s="5"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
@@ -15229,7 +15282,7 @@
       <c r="Q54" s="1"/>
       <c r="R54" s="6"/>
     </row>
-    <row r="55" spans="2:18">
+    <row r="55" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B55" s="5"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
@@ -15248,7 +15301,7 @@
       <c r="Q55" s="1"/>
       <c r="R55" s="6"/>
     </row>
-    <row r="56" spans="2:18">
+    <row r="56" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B56" s="5"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
@@ -15267,7 +15320,7 @@
       <c r="Q56" s="1"/>
       <c r="R56" s="6"/>
     </row>
-    <row r="57" spans="2:18">
+    <row r="57" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B57" s="5"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
@@ -15286,7 +15339,7 @@
       <c r="Q57" s="1"/>
       <c r="R57" s="6"/>
     </row>
-    <row r="58" spans="2:18">
+    <row r="58" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B58" s="5"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
@@ -15305,7 +15358,7 @@
       <c r="Q58" s="1"/>
       <c r="R58" s="6"/>
     </row>
-    <row r="59" spans="2:18">
+    <row r="59" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B59" s="5"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
@@ -15324,7 +15377,7 @@
       <c r="Q59" s="1"/>
       <c r="R59" s="6"/>
     </row>
-    <row r="60" spans="2:18">
+    <row r="60" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B60" s="5"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
@@ -15343,7 +15396,7 @@
       <c r="Q60" s="1"/>
       <c r="R60" s="6"/>
     </row>
-    <row r="61" spans="2:18">
+    <row r="61" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B61" s="5"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
@@ -15362,7 +15415,7 @@
       <c r="Q61" s="1"/>
       <c r="R61" s="6"/>
     </row>
-    <row r="62" spans="2:18">
+    <row r="62" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B62" s="5"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
@@ -15380,7 +15433,7 @@
       <c r="Q62" s="1"/>
       <c r="R62" s="6"/>
     </row>
-    <row r="63" spans="2:18">
+    <row r="63" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B63" s="5"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
@@ -15399,7 +15452,7 @@
       <c r="Q63" s="1"/>
       <c r="R63" s="6"/>
     </row>
-    <row r="64" spans="2:18">
+    <row r="64" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B64" s="5"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
@@ -15418,7 +15471,7 @@
       <c r="Q64" s="1"/>
       <c r="R64" s="6"/>
     </row>
-    <row r="65" spans="2:18">
+    <row r="65" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B65" s="5"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
@@ -15437,7 +15490,7 @@
       <c r="Q65" s="1"/>
       <c r="R65" s="6"/>
     </row>
-    <row r="66" spans="2:18">
+    <row r="66" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B66" s="5"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
@@ -15456,7 +15509,7 @@
       <c r="Q66" s="1"/>
       <c r="R66" s="6"/>
     </row>
-    <row r="67" spans="2:18">
+    <row r="67" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B67" s="5"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
@@ -15475,7 +15528,7 @@
       <c r="Q67" s="1"/>
       <c r="R67" s="6"/>
     </row>
-    <row r="68" spans="2:18">
+    <row r="68" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B68" s="5"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
@@ -15494,7 +15547,7 @@
       <c r="Q68" s="1"/>
       <c r="R68" s="6"/>
     </row>
-    <row r="69" spans="2:18">
+    <row r="69" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B69" s="5"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
@@ -15513,7 +15566,7 @@
       <c r="Q69" s="1"/>
       <c r="R69" s="6"/>
     </row>
-    <row r="70" spans="2:18">
+    <row r="70" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B70" s="5"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
@@ -15532,7 +15585,7 @@
       <c r="Q70" s="1"/>
       <c r="R70" s="6"/>
     </row>
-    <row r="71" spans="2:18">
+    <row r="71" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B71" s="5"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
@@ -15551,7 +15604,7 @@
       <c r="Q71" s="1"/>
       <c r="R71" s="6"/>
     </row>
-    <row r="72" spans="2:18">
+    <row r="72" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B72" s="5"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
@@ -15570,7 +15623,7 @@
       <c r="Q72" s="1"/>
       <c r="R72" s="6"/>
     </row>
-    <row r="73" spans="2:18">
+    <row r="73" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B73" s="5"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
@@ -15589,7 +15642,7 @@
       <c r="Q73" s="1"/>
       <c r="R73" s="6"/>
     </row>
-    <row r="74" spans="2:18">
+    <row r="74" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B74" s="5"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
@@ -15608,7 +15661,7 @@
       <c r="Q74" s="1"/>
       <c r="R74" s="6"/>
     </row>
-    <row r="75" spans="2:18">
+    <row r="75" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B75" s="5"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
@@ -15627,7 +15680,7 @@
       <c r="Q75" s="1"/>
       <c r="R75" s="6"/>
     </row>
-    <row r="76" spans="2:18">
+    <row r="76" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B76" s="5"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
@@ -15646,7 +15699,7 @@
       <c r="Q76" s="1"/>
       <c r="R76" s="6"/>
     </row>
-    <row r="77" spans="2:18">
+    <row r="77" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B77" s="5"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
@@ -15665,7 +15718,7 @@
       <c r="Q77" s="1"/>
       <c r="R77" s="6"/>
     </row>
-    <row r="78" spans="2:18">
+    <row r="78" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B78" s="5"/>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
@@ -15684,7 +15737,7 @@
       <c r="Q78" s="1"/>
       <c r="R78" s="6"/>
     </row>
-    <row r="79" spans="2:18">
+    <row r="79" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B79" s="7"/>
       <c r="C79" s="8"/>
       <c r="D79" s="8"/>
@@ -15718,4 +15771,88 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AB37B1D-1558-41D3-9521-7BA857188B96}">
+  <dimension ref="D7:J10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="9.140625" style="39"/>
+    <col min="5" max="5" width="15.28515625" style="39" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="9.140625" style="39"/>
+    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="7" spans="4:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D7" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="43" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="I7" s="43" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" s="43" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="4:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D8" s="40">
+        <v>1</v>
+      </c>
+      <c r="E8" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="41"/>
+    </row>
+    <row r="9" spans="4:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D9" s="40">
+        <v>2</v>
+      </c>
+      <c r="E9" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="41"/>
+    </row>
+    <row r="10" spans="4:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D10" s="42">
+        <v>3</v>
+      </c>
+      <c r="E10" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="44"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>